<commit_message>
Update office location  and contact transfer scenario
</commit_message>
<xml_diff>
--- a/SmokeTestCases.xlsx
+++ b/SmokeTestCases.xlsx
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="945" uniqueCount="515">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1571" uniqueCount="538">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -1613,6 +1613,75 @@
   </si>
   <si>
     <t>6/15/2022</t>
+  </si>
+  <si>
+    <t>6/18/2022</t>
+  </si>
+  <si>
+    <t>DD-0219</t>
+  </si>
+  <si>
+    <t>DD-0220</t>
+  </si>
+  <si>
+    <t>DD-0221</t>
+  </si>
+  <si>
+    <t>DD-0222</t>
+  </si>
+  <si>
+    <t>DD-0223</t>
+  </si>
+  <si>
+    <t>DD-0224</t>
+  </si>
+  <si>
+    <t>CC-0662</t>
+  </si>
+  <si>
+    <t>CC-0663</t>
+  </si>
+  <si>
+    <t>CC-0664</t>
+  </si>
+  <si>
+    <t>CC-0665</t>
+  </si>
+  <si>
+    <t>CC-0666</t>
+  </si>
+  <si>
+    <t>FD-0232</t>
+  </si>
+  <si>
+    <t>ID-0644</t>
+  </si>
+  <si>
+    <t>ID-0645</t>
+  </si>
+  <si>
+    <t>ID-0646</t>
+  </si>
+  <si>
+    <t>ID-0647</t>
+  </si>
+  <si>
+    <t>FD-0233</t>
+  </si>
+  <si>
+    <t>ID-0648</t>
+  </si>
+  <si>
+    <t>ID-0649</t>
+  </si>
+  <si>
+    <t>ID-0650</t>
+  </si>
+  <si>
+    <t>ID-0651</t>
+  </si>
+  <si>
+    <t>ID-0652</t>
   </si>
 </sst>
 </file>
@@ -2889,7 +2958,7 @@
         <v>370</v>
       </c>
       <c r="B9" t="s">
-        <v>425</v>
+        <v>497</v>
       </c>
       <c r="C9" t="s">
         <v>246</v>
@@ -2907,7 +2976,7 @@
         <v>280</v>
       </c>
       <c r="H9" t="s">
-        <v>456</v>
+        <v>495</v>
       </c>
       <c r="K9" s="14" t="s">
         <v>374</v>
@@ -3073,10 +3142,10 @@
         <v>302</v>
       </c>
       <c r="B2" t="s">
-        <v>432</v>
+        <v>522</v>
       </c>
       <c r="C2" t="s">
-        <v>431</v>
+        <v>521</v>
       </c>
       <c r="D2" t="s">
         <v>502</v>
@@ -3094,10 +3163,10 @@
         <v>380</v>
       </c>
       <c r="I2" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="J2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="K2" s="15" t="s">
         <v>374</v>
@@ -3114,10 +3183,10 @@
         <v>303</v>
       </c>
       <c r="B3" t="s">
-        <v>433</v>
+        <v>523</v>
       </c>
       <c r="C3" t="s">
-        <v>431</v>
+        <v>521</v>
       </c>
       <c r="D3" t="s">
         <v>498</v>
@@ -3135,10 +3204,10 @@
         <v>377</v>
       </c>
       <c r="I3" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="J3" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="K3" s="15" t="s">
         <v>229</v>
@@ -3155,10 +3224,10 @@
         <v>304</v>
       </c>
       <c r="B4" t="s">
-        <v>434</v>
+        <v>524</v>
       </c>
       <c r="C4" t="s">
-        <v>431</v>
+        <v>521</v>
       </c>
       <c r="D4" t="s">
         <v>497</v>
@@ -3176,16 +3245,16 @@
         <v>374</v>
       </c>
       <c r="I4" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="J4" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="K4" t="s">
         <v>374</v>
       </c>
       <c r="L4" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="M4" t="s">
         <v>356</v>
@@ -3196,10 +3265,10 @@
         <v>305</v>
       </c>
       <c r="B5" t="s">
-        <v>435</v>
+        <v>525</v>
       </c>
       <c r="C5" t="s">
-        <v>431</v>
+        <v>521</v>
       </c>
       <c r="D5" t="s">
         <v>503</v>
@@ -3217,10 +3286,10 @@
         <v>382</v>
       </c>
       <c r="I5" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="J5" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="K5" s="14" t="s">
         <v>229</v>
@@ -3237,10 +3306,10 @@
         <v>306</v>
       </c>
       <c r="B6" t="s">
-        <v>436</v>
+        <v>526</v>
       </c>
       <c r="C6" t="s">
-        <v>431</v>
+        <v>521</v>
       </c>
       <c r="D6" t="s">
         <v>506</v>
@@ -3258,10 +3327,10 @@
         <v>429</v>
       </c>
       <c r="I6" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="J6" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="K6" s="15" t="s">
         <v>229</v>
@@ -3352,7 +3421,7 @@
         <v>291</v>
       </c>
       <c r="B2" t="s">
-        <v>431</v>
+        <v>521</v>
       </c>
       <c r="C2" t="s">
         <v>71</v>
@@ -3361,10 +3430,10 @@
         <v>384</v>
       </c>
       <c r="E2" t="s">
-        <v>496</v>
+        <v>501</v>
       </c>
       <c r="F2" t="s">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="G2" s="14">
         <v>5500000</v>
@@ -3464,7 +3533,7 @@
         <v>406</v>
       </c>
       <c r="B2" t="s">
-        <v>450</v>
+        <v>532</v>
       </c>
       <c r="D2">
         <v>15000000</v>
@@ -3550,31 +3619,31 @@
         <v>401</v>
       </c>
       <c r="B2" t="s">
-        <v>450</v>
+        <v>532</v>
       </c>
       <c r="C2" t="s">
-        <v>451</v>
+        <v>533</v>
       </c>
       <c r="D2" t="s">
-        <v>422</v>
+        <v>502</v>
       </c>
       <c r="E2" t="s">
-        <v>437</v>
+        <v>444</v>
       </c>
       <c r="F2" t="s">
-        <v>438</v>
+        <v>445</v>
       </c>
       <c r="G2" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="H2" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="I2" t="s">
-        <v>439</v>
+        <v>446</v>
       </c>
       <c r="J2" t="s">
-        <v>440</v>
+        <v>447</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
@@ -3582,31 +3651,31 @@
         <v>402</v>
       </c>
       <c r="B3" t="s">
-        <v>450</v>
+        <v>532</v>
       </c>
       <c r="C3" t="s">
-        <v>452</v>
+        <v>534</v>
       </c>
       <c r="D3" t="s">
-        <v>423</v>
+        <v>498</v>
       </c>
       <c r="E3" t="s">
-        <v>438</v>
+        <v>420</v>
       </c>
       <c r="F3" t="s">
-        <v>377</v>
+        <v>374</v>
       </c>
       <c r="G3" t="s">
-        <v>441</v>
+        <v>448</v>
       </c>
       <c r="H3" t="s">
-        <v>441</v>
+        <v>448</v>
       </c>
       <c r="I3" t="s">
-        <v>441</v>
+        <v>448</v>
       </c>
       <c r="J3" t="s">
-        <v>442</v>
+        <v>449</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
@@ -3614,13 +3683,13 @@
         <v>403</v>
       </c>
       <c r="B4" t="s">
-        <v>450</v>
+        <v>532</v>
       </c>
       <c r="C4" t="s">
-        <v>453</v>
+        <v>535</v>
       </c>
       <c r="D4" t="s">
-        <v>425</v>
+        <v>497</v>
       </c>
       <c r="E4" t="s">
         <v>419</v>
@@ -3646,31 +3715,31 @@
         <v>404</v>
       </c>
       <c r="B5" t="s">
-        <v>450</v>
+        <v>532</v>
       </c>
       <c r="C5" t="s">
-        <v>454</v>
+        <v>536</v>
       </c>
       <c r="D5" t="s">
-        <v>421</v>
+        <v>503</v>
       </c>
       <c r="E5" t="s">
-        <v>444</v>
+        <v>437</v>
       </c>
       <c r="F5" t="s">
-        <v>445</v>
+        <v>438</v>
       </c>
       <c r="G5" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="H5" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="I5" t="s">
-        <v>446</v>
+        <v>439</v>
       </c>
       <c r="J5" t="s">
-        <v>447</v>
+        <v>440</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
@@ -3678,31 +3747,31 @@
         <v>405</v>
       </c>
       <c r="B6" t="s">
-        <v>450</v>
+        <v>532</v>
       </c>
       <c r="C6" t="s">
-        <v>455</v>
+        <v>537</v>
       </c>
       <c r="D6" t="s">
-        <v>426</v>
+        <v>506</v>
       </c>
       <c r="E6" t="s">
-        <v>420</v>
+        <v>438</v>
       </c>
       <c r="F6" t="s">
-        <v>374</v>
+        <v>377</v>
       </c>
       <c r="G6" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="H6" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="I6" t="s">
-        <v>448</v>
+        <v>441</v>
       </c>
       <c r="J6" t="s">
-        <v>449</v>
+        <v>442</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
OLD SMOKE PE SCRIPT UPDATION.
Signed-off-by: sahilnavatar <106244111+sahilnavatar@users.noreply.github.com>
</commit_message>
<xml_diff>
--- a/SmokeTestCases.xlsx
+++ b/SmokeTestCases.xlsx
@@ -1,32 +1,35 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" tabRatio="622" activeTab="1"/>
+    <workbookView activeTab="18" firstSheet="13" tabRatio="622" windowHeight="11160" windowWidth="20730" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
-    <sheet name="Institutions" sheetId="22" r:id="rId1"/>
-    <sheet name="Limited Partner" sheetId="26" r:id="rId2"/>
-    <sheet name="Fundraising Contacts" sheetId="34" r:id="rId3"/>
-    <sheet name="Contacts" sheetId="23" r:id="rId4"/>
-    <sheet name="Funds" sheetId="27" r:id="rId5"/>
-    <sheet name="Fundraisings" sheetId="24" r:id="rId6"/>
-    <sheet name="MI" sheetId="33" r:id="rId7"/>
-    <sheet name="PipeLine" sheetId="37" r:id="rId8"/>
-    <sheet name="Office Location" sheetId="38" r:id="rId9"/>
-    <sheet name="Partnerships" sheetId="28" r:id="rId10"/>
-    <sheet name="Commitments" sheetId="25" r:id="rId11"/>
-    <sheet name="CapitalCall" sheetId="40" r:id="rId12"/>
-    <sheet name="FundDrawdown" sheetId="41" r:id="rId13"/>
-    <sheet name="FundDistribution" sheetId="42" r:id="rId14"/>
-    <sheet name="InvestorDistribution" sheetId="43" r:id="rId15"/>
-    <sheet name="Activities" sheetId="39" r:id="rId16"/>
-    <sheet name="Users" sheetId="29" r:id="rId17"/>
-    <sheet name="CustomEmailFolder" sheetId="35" r:id="rId18"/>
-    <sheet name="Report" sheetId="36" r:id="rId19"/>
+    <sheet name="Institutions" r:id="rId1" sheetId="22"/>
+    <sheet name="Limited Partner" r:id="rId2" sheetId="26"/>
+    <sheet name="Fundraising Contacts" r:id="rId3" sheetId="34"/>
+    <sheet name="Contacts" r:id="rId4" sheetId="23"/>
+    <sheet name="Funds" r:id="rId5" sheetId="27"/>
+    <sheet name="Fundraisings" r:id="rId6" sheetId="24"/>
+    <sheet name="MI" r:id="rId7" sheetId="33"/>
+    <sheet name="PipeLine" r:id="rId8" sheetId="37"/>
+    <sheet name="Office Location" r:id="rId9" sheetId="38"/>
+    <sheet name="Partnerships" r:id="rId10" sheetId="28"/>
+    <sheet name="Commitments" r:id="rId11" sheetId="25"/>
+    <sheet name="CapitalCall" r:id="rId12" sheetId="40"/>
+    <sheet name="FundDrawdown" r:id="rId13" sheetId="41"/>
+    <sheet name="FundDistribution" r:id="rId14" sheetId="42"/>
+    <sheet name="InvestorDistribution" r:id="rId15" sheetId="43"/>
+    <sheet name="Activities" r:id="rId16" sheetId="39"/>
+    <sheet name="Users" r:id="rId17" sheetId="29"/>
+    <sheet name="CustomEmailFolder" r:id="rId18" sheetId="35"/>
+    <sheet name="Report" r:id="rId19" sheetId="36"/>
   </sheets>
+  <definedNames>
+    <definedName hidden="1" localSheetId="2" name="_xlnm._FilterDatabase">'Fundraising Contacts'!$A$1:$J$9</definedName>
+  </definedNames>
   <calcPr calcId="125725"/>
   <fileRecoveryPr autoRecover="0"/>
 </workbook>
@@ -38,7 +41,7 @@
     <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="C6" authorId="0" shapeId="0">
+    <comment authorId="0" ref="C6" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -68,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="871" uniqueCount="505">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="487">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -1336,30 +1339,9 @@
     <t>10000000</t>
   </si>
   <si>
-    <t>CMT - 000932</t>
-  </si>
-  <si>
-    <t>CMT - 000933</t>
-  </si>
-  <si>
-    <t>CMT - 000934</t>
-  </si>
-  <si>
-    <t>CMT - 000935</t>
-  </si>
-  <si>
-    <t>CMT - 000936</t>
-  </si>
-  <si>
     <t>3/20/2020</t>
   </si>
   <si>
-    <t>CMT - 000930</t>
-  </si>
-  <si>
-    <t>CMT - 000931</t>
-  </si>
-  <si>
     <t>400000</t>
   </si>
   <si>
@@ -1372,18 +1354,6 @@
     <t>500,000.000</t>
   </si>
   <si>
-    <t>DD-0215</t>
-  </si>
-  <si>
-    <t>CC-0619</t>
-  </si>
-  <si>
-    <t>CC-0620</t>
-  </si>
-  <si>
-    <t>CC-0621</t>
-  </si>
-  <si>
     <t>CC-0622</t>
   </si>
   <si>
@@ -1429,51 +1399,12 @@
     <t>2399999.999</t>
   </si>
   <si>
-    <t>FD-0228</t>
-  </si>
-  <si>
-    <t>ID-0625</t>
-  </si>
-  <si>
-    <t>ID-0626</t>
-  </si>
-  <si>
-    <t>ID-0627</t>
-  </si>
-  <si>
     <t>ID-0628</t>
   </si>
   <si>
     <t>ID-0629</t>
   </si>
   <si>
-    <t>7/20/2020</t>
-  </si>
-  <si>
-    <t>7/21/2020</t>
-  </si>
-  <si>
-    <t>7/23/2020</t>
-  </si>
-  <si>
-    <t>7/24/2020</t>
-  </si>
-  <si>
-    <t>7/27/2020</t>
-  </si>
-  <si>
-    <t>7/30/2020</t>
-  </si>
-  <si>
-    <t>4.2E7</t>
-  </si>
-  <si>
-    <t>8/4/2020</t>
-  </si>
-  <si>
-    <t>TestCompany1 - Jul 2020</t>
-  </si>
-  <si>
     <t>TestCompany2 - Jul 2020</t>
   </si>
   <si>
@@ -1498,91 +1429,109 @@
     <t>All firms</t>
   </si>
   <si>
-    <t>CustomReportFolder96907</t>
-  </si>
-  <si>
-    <t>CustomReport21177</t>
-  </si>
-  <si>
-    <t>PETestEmailFolder59988</t>
-  </si>
-  <si>
-    <t>PETestCustomEmailTemplate29575</t>
-  </si>
-  <si>
-    <t>deelroom+23257@gmail.com</t>
-  </si>
-  <si>
-    <t>deelroom+23771@gmail.com</t>
-  </si>
-  <si>
-    <t>deelroom+15617@gmail.com</t>
-  </si>
-  <si>
-    <t>deelroom+42061@gmail.com</t>
-  </si>
-  <si>
-    <t>deelroom+72853@gmail.com</t>
-  </si>
-  <si>
     <t>2/16/2022</t>
   </si>
   <si>
-    <t>4.8E8</t>
-  </si>
-  <si>
-    <t>2/18/2022</t>
-  </si>
-  <si>
-    <t>CMT - 000962</t>
-  </si>
-  <si>
-    <t>CMT - 000963</t>
-  </si>
-  <si>
-    <t>5.2E8</t>
-  </si>
-  <si>
-    <t>2/20/2022</t>
-  </si>
-  <si>
-    <t>2/21/2022</t>
-  </si>
-  <si>
-    <t>CMT - 000965</t>
-  </si>
-  <si>
-    <t>CMT - 000966</t>
-  </si>
-  <si>
-    <t>5.25E8</t>
-  </si>
-  <si>
-    <t>2/24/2022</t>
-  </si>
-  <si>
-    <t>CMT - 000967</t>
-  </si>
-  <si>
-    <t>4.4E7</t>
-  </si>
-  <si>
-    <t>2/27/2022</t>
-  </si>
-  <si>
-    <t>CMT - 000968</t>
-  </si>
-  <si>
-    <t>5.6E7</t>
-  </si>
-  <si>
-    <t>3/4/2022</t>
-  </si>
-  <si>
-    <t>CMT - 000969</t>
-  </si>
-  <si>
     <t>TestCompany1 - Feb 2022</t>
+  </si>
+  <si>
+    <t>PETestEmailFolder90700</t>
+  </si>
+  <si>
+    <t>PETestCustomEmailTemplate25516</t>
+  </si>
+  <si>
+    <t>navatariptesting+84488@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+14032@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+49277@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+54430@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+40025@gmail.com</t>
+  </si>
+  <si>
+    <t>7/20/2022</t>
+  </si>
+  <si>
+    <t>7/21/2022</t>
+  </si>
+  <si>
+    <t>CMT - 000952</t>
+  </si>
+  <si>
+    <t>CMT - 000953</t>
+  </si>
+  <si>
+    <t>7/23/2022</t>
+  </si>
+  <si>
+    <t>7/24/2022</t>
+  </si>
+  <si>
+    <t>CMT - 000954</t>
+  </si>
+  <si>
+    <t>CMT - 000955</t>
+  </si>
+  <si>
+    <t>6.0E8</t>
+  </si>
+  <si>
+    <t>7/27/2022</t>
+  </si>
+  <si>
+    <t>CMT - 000956</t>
+  </si>
+  <si>
+    <t>7/30/2022</t>
+  </si>
+  <si>
+    <t>CMT - 000957</t>
+  </si>
+  <si>
+    <t>7.0E7</t>
+  </si>
+  <si>
+    <t>8/4/2022</t>
+  </si>
+  <si>
+    <t>CMT - 000958</t>
+  </si>
+  <si>
+    <t>DD-0216</t>
+  </si>
+  <si>
+    <t>CC-0624</t>
+  </si>
+  <si>
+    <t>CC-0625</t>
+  </si>
+  <si>
+    <t>CC-0626</t>
+  </si>
+  <si>
+    <t>FD-0229</t>
+  </si>
+  <si>
+    <t>ID-0630</t>
+  </si>
+  <si>
+    <t>ID-0631</t>
+  </si>
+  <si>
+    <t>ID-0632</t>
+  </si>
+  <si>
+    <t>CustomReportFolder47527</t>
+  </si>
+  <si>
+    <t>CustomReport57424</t>
   </si>
 </sst>
 </file>
@@ -1590,8 +1539,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
-    <numFmt numFmtId="165" formatCode="mm/dd/yy;@"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+    <numFmt numFmtId="164" formatCode="mm/dd/yy;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -1662,72 +1611,72 @@
     </border>
   </borders>
   <cellStyleXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="1" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="29">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="1" numFmtId="0" xfId="1"/>
+    <xf applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyFill="1" borderId="0" fillId="2" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="2" numFmtId="164" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="164" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFont="1" borderId="0" fillId="0" fontId="2" numFmtId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="2" numFmtId="49" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" quotePrefix="1" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="2" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="8" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="9" xfId="0"/>
+    <xf applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="2" numFmtId="49" xfId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" quotePrefix="1" xfId="0"/>
+    <xf applyFont="1" applyNumberFormat="1" borderId="0" fillId="0" fontId="5" numFmtId="14" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" applyNumberFormat="1" borderId="0" fillId="2" fontId="2" numFmtId="2" xfId="0">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" xfId="0"/>
+    <xf applyNumberFormat="1" borderId="0" fillId="0" fontId="0" numFmtId="2" quotePrefix="1" xfId="0"/>
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" applyFill="1" applyFont="1" borderId="0" fillId="2" fontId="2" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="8" name="Hyperlink" xfId="1"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <colors>
     <mruColors>
       <color rgb="FFFFABAB"/>
@@ -1749,10 +1698,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1916,21 +1865,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="6350" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="6350">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1947,7 +1896,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -1999,48 +1948,48 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" name="Office Theme" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:W15"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:X15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C21" sqref="C21"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="A9" pane="bottomLeft" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" customWidth="true" width="24.7265625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="20.453125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="43.26953125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="43.1796875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="22.7265625" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="14.1796875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="26.26953125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="24.453125" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.7265625" collapsed="true"/>
-    <col min="11" max="11" customWidth="true" width="20.453125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="17.81640625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.1796875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="15.54296875" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="8.453125" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="15.1796875" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="13.1796875" collapsed="true"/>
+    <col min="1" max="1" customWidth="true" width="24.7109375" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="43.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="43.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="22.7109375" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="14.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="24.42578125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
+    <col min="11" max="11" customWidth="true" width="20.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="17.85546875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.140625" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="8.42578125" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="13.140625" collapsed="true"/>
     <col min="19" max="19" customWidth="true" width="20.0" collapsed="true"/>
-    <col min="20" max="20" customWidth="true" width="17.453125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="17.453125" collapsed="true"/>
+    <col min="20" max="20" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
     <col min="22" max="22" bestFit="true" customWidth="true" width="11.0" collapsed="true"/>
     <col min="23" max="23" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:23" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="1" s="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
@@ -2111,7 +2060,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="2" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>91</v>
       </c>
@@ -2122,7 +2071,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>92</v>
       </c>
@@ -2154,7 +2103,7 @@
         <v>554477331</v>
       </c>
     </row>
-    <row r="4" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>93</v>
       </c>
@@ -2165,7 +2114,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>94</v>
       </c>
@@ -2197,7 +2146,7 @@
         <v>330548934</v>
       </c>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>95</v>
       </c>
@@ -2208,7 +2157,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>97</v>
       </c>
@@ -2219,7 +2168,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>99</v>
       </c>
@@ -2230,7 +2179,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>100</v>
       </c>
@@ -2241,7 +2190,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>96</v>
       </c>
@@ -2252,7 +2201,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>98</v>
       </c>
@@ -2263,7 +2212,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>341</v>
       </c>
@@ -2322,7 +2271,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>342</v>
       </c>
@@ -2378,7 +2327,7 @@
         <v>98765429</v>
       </c>
     </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>343</v>
       </c>
@@ -2434,7 +2383,7 @@
         <v>1629539588</v>
       </c>
     </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>344</v>
       </c>
@@ -2495,31 +2444,31 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E15" r:id="rId1"/>
+    <hyperlink r:id="rId1" ref="E15"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C18" sqref="C18"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="C18" pane="bottomLeft" sqref="C18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="26.1796875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="26.140625" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
     <col min="4" max="4" customWidth="true" width="24.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="1" s="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2533,7 +2482,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>260</v>
       </c>
@@ -2544,7 +2493,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>262</v>
       </c>
@@ -2558,7 +2507,7 @@
         <v>289</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>264</v>
       </c>
@@ -2569,7 +2518,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>266</v>
       </c>
@@ -2581,44 +2530,44 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:T10"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:U10"/>
   <sheetViews>
     <sheetView topLeftCell="M1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="S1" sqref="S1"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="S1" pane="bottomLeft" sqref="S1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="15.7265625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="23.81640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="25.26953125" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="23.1796875" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="13.26953125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="9.81640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="22.453125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="16.81640625" collapsed="true"/>
-    <col min="10" max="10" customWidth="true" width="18.453125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" style="15" width="19.26953125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="23.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="25.28515625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="9.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="16.85546875" collapsed="true"/>
+    <col min="10" max="10" customWidth="true" width="18.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" style="15" width="19.28515625" collapsed="true"/>
     <col min="12" max="12" bestFit="true" customWidth="true" style="15" width="22.0" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" style="15" width="21.54296875" collapsed="true"/>
-    <col min="14" max="14" customWidth="true" style="15" width="22.54296875" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" style="15" width="21.5703125" collapsed="true"/>
+    <col min="14" max="14" customWidth="true" style="15" width="22.5703125" collapsed="true"/>
     <col min="15" max="15" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="16" max="16" customWidth="true" width="13.54296875" collapsed="true"/>
-    <col min="17" max="17" customWidth="true" width="21.453125" collapsed="true"/>
-    <col min="18" max="18" customWidth="true" width="35.1796875" collapsed="true"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" width="33.54296875" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="16.54296875" collapsed="true"/>
+    <col min="16" max="16" customWidth="true" width="13.5703125" collapsed="true"/>
+    <col min="17" max="17" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="18" max="18" customWidth="true" width="35.140625" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" width="33.5703125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:20" s="1" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" customHeight="1" ht="15.75" r="1" s="1" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -2680,12 +2629,12 @@
         <v>278</v>
       </c>
     </row>
-    <row r="2" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>279</v>
       </c>
       <c r="B2" t="s">
-        <v>488</v>
+        <v>463</v>
       </c>
       <c r="C2" t="s">
         <v>247</v>
@@ -2703,19 +2652,19 @@
         <v>281</v>
       </c>
       <c r="H2" t="s">
-        <v>485</v>
+        <v>461</v>
       </c>
       <c r="P2" s="18"/>
       <c r="T2" s="28" t="s">
         <v>248</v>
       </c>
     </row>
-    <row r="3" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>282</v>
       </c>
       <c r="B3" t="s">
-        <v>489</v>
+        <v>464</v>
       </c>
       <c r="C3" t="s">
         <v>250</v>
@@ -2733,16 +2682,16 @@
         <v>281</v>
       </c>
       <c r="H3" t="s">
-        <v>487</v>
+        <v>462</v>
       </c>
       <c r="T3" s="28"/>
     </row>
-    <row r="4" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>287</v>
       </c>
       <c r="B4" t="s">
-        <v>493</v>
+        <v>467</v>
       </c>
       <c r="C4" t="s">
         <v>247</v>
@@ -2754,19 +2703,19 @@
         <v>15000000</v>
       </c>
       <c r="H4" t="s">
-        <v>491</v>
+        <v>465</v>
       </c>
       <c r="J4">
         <v>7.5</v>
       </c>
       <c r="T4" s="28"/>
     </row>
-    <row r="5" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>288</v>
       </c>
       <c r="B5" t="s">
-        <v>494</v>
+        <v>468</v>
       </c>
       <c r="C5" t="s">
         <v>252</v>
@@ -2778,19 +2727,19 @@
         <v>25000000</v>
       </c>
       <c r="H5" t="s">
-        <v>492</v>
+        <v>466</v>
       </c>
       <c r="J5">
         <v>7.5</v>
       </c>
       <c r="T5" s="28"/>
     </row>
-    <row r="6" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>290</v>
       </c>
       <c r="B6" t="s">
-        <v>497</v>
+        <v>471</v>
       </c>
       <c r="C6" t="s">
         <v>255</v>
@@ -2802,16 +2751,16 @@
         <v>5000000</v>
       </c>
       <c r="H6" t="s">
-        <v>496</v>
+        <v>470</v>
       </c>
       <c r="T6" s="28"/>
     </row>
-    <row r="7" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>310</v>
       </c>
       <c r="B7" t="s">
-        <v>500</v>
+        <v>473</v>
       </c>
       <c r="C7" t="s">
         <v>255</v>
@@ -2823,19 +2772,19 @@
         <v>2000000</v>
       </c>
       <c r="H7" t="s">
-        <v>499</v>
+        <v>472</v>
       </c>
       <c r="I7" t="s">
         <v>40</v>
       </c>
       <c r="T7" s="28"/>
     </row>
-    <row r="8" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>388</v>
       </c>
       <c r="B8" t="s">
-        <v>503</v>
+        <v>476</v>
       </c>
       <c r="C8" t="s">
         <v>257</v>
@@ -2847,19 +2796,19 @@
         <v>12000000</v>
       </c>
       <c r="H8" t="s">
-        <v>502</v>
+        <v>475</v>
       </c>
       <c r="I8" t="s">
         <v>40</v>
       </c>
       <c r="T8" s="28"/>
     </row>
-    <row r="9" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>371</v>
       </c>
       <c r="B9" t="s">
-        <v>428</v>
+        <v>463</v>
       </c>
       <c r="C9" t="s">
         <v>247</v>
@@ -2877,7 +2826,7 @@
         <v>281</v>
       </c>
       <c r="H9" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="K9" s="14" t="s">
         <v>375</v>
@@ -2910,7 +2859,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="10" spans="1:20" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>285</v>
       </c>
@@ -2970,34 +2919,34 @@
   <mergeCells count="1">
     <mergeCell ref="T2:T8"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="12.81640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.26953125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="19.81640625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="13.453125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="13.42578125" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -3038,18 +2987,18 @@
         <v>302</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
         <v>303</v>
       </c>
       <c r="B2" t="s">
-        <v>435</v>
+        <v>427</v>
       </c>
       <c r="C2" t="s">
-        <v>434</v>
+        <v>477</v>
       </c>
       <c r="D2" t="s">
-        <v>423</v>
+        <v>468</v>
       </c>
       <c r="E2" t="s">
         <v>375</v>
@@ -3064,10 +3013,10 @@
         <v>383</v>
       </c>
       <c r="I2" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="J2" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="K2" s="15" t="s">
         <v>375</v>
@@ -3079,36 +3028,36 @@
         <v>362</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>304</v>
       </c>
       <c r="B3" t="s">
-        <v>436</v>
+        <v>428</v>
       </c>
       <c r="C3" t="s">
-        <v>434</v>
+        <v>477</v>
       </c>
       <c r="D3" t="s">
+        <v>471</v>
+      </c>
+      <c r="E3" t="s">
+        <v>423</v>
+      </c>
+      <c r="F3" t="s">
         <v>424</v>
       </c>
-      <c r="E3" t="s">
-        <v>430</v>
-      </c>
-      <c r="F3" t="s">
-        <v>431</v>
-      </c>
       <c r="G3" t="s">
-        <v>431</v>
+        <v>424</v>
       </c>
       <c r="H3" t="s">
-        <v>432</v>
+        <v>425</v>
       </c>
       <c r="I3" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="J3" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="K3" s="15" t="s">
         <v>230</v>
@@ -3117,21 +3066,21 @@
         <v>360</v>
       </c>
       <c r="M3" t="s">
-        <v>433</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>305</v>
       </c>
       <c r="B4" t="s">
-        <v>437</v>
+        <v>478</v>
       </c>
       <c r="C4" t="s">
-        <v>434</v>
+        <v>477</v>
       </c>
       <c r="D4" t="s">
-        <v>428</v>
+        <v>463</v>
       </c>
       <c r="E4" t="s">
         <v>373</v>
@@ -3146,51 +3095,51 @@
         <v>375</v>
       </c>
       <c r="I4" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="J4" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="K4" t="s">
         <v>375</v>
       </c>
       <c r="L4" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="M4" t="s">
         <v>357</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>306</v>
       </c>
       <c r="B5" t="s">
-        <v>438</v>
+        <v>479</v>
       </c>
       <c r="C5" t="s">
-        <v>434</v>
+        <v>477</v>
       </c>
       <c r="D5" t="s">
-        <v>422</v>
+        <v>464</v>
       </c>
       <c r="E5" t="s">
-        <v>379</v>
+        <v>376</v>
       </c>
       <c r="F5" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="G5" t="s">
-        <v>380</v>
+        <v>377</v>
       </c>
       <c r="H5" t="s">
-        <v>381</v>
+        <v>378</v>
       </c>
       <c r="I5" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="J5" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="K5" s="14" t="s">
         <v>230</v>
@@ -3199,39 +3148,39 @@
         <v>363</v>
       </c>
       <c r="M5" t="s">
-        <v>361</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>307</v>
       </c>
       <c r="B6" t="s">
-        <v>439</v>
+        <v>480</v>
       </c>
       <c r="C6" t="s">
-        <v>434</v>
+        <v>477</v>
       </c>
       <c r="D6" t="s">
-        <v>429</v>
+        <v>467</v>
       </c>
       <c r="E6" t="s">
-        <v>376</v>
+        <v>379</v>
       </c>
       <c r="F6" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="G6" t="s">
-        <v>377</v>
+        <v>380</v>
       </c>
       <c r="H6" t="s">
-        <v>378</v>
+        <v>381</v>
       </c>
       <c r="I6" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="J6" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="K6" s="15" t="s">
         <v>230</v>
@@ -3240,37 +3189,37 @@
         <v>364</v>
       </c>
       <c r="M6" t="s">
-        <v>359</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="12.453125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="9.453125" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="19.26953125" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="23.1796875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="19.453125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="12.42578125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="19.28515625" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="19.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3317,12 +3266,12 @@
         <v>394</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>292</v>
       </c>
       <c r="B2" t="s">
-        <v>434</v>
+        <v>477</v>
       </c>
       <c r="C2" t="s">
         <v>72</v>
@@ -3331,10 +3280,10 @@
         <v>385</v>
       </c>
       <c r="E2" t="s">
-        <v>459</v>
+        <v>461</v>
       </c>
       <c r="F2" t="s">
-        <v>460</v>
+        <v>462</v>
       </c>
       <c r="G2" s="14">
         <v>5500000</v>
@@ -3365,30 +3314,30 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:N2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.1796875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.453125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="12.7265625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="16.26953125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="11.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.42578125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="16.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3429,12 +3378,12 @@
         <v>394</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>407</v>
       </c>
       <c r="B2" t="s">
-        <v>453</v>
+        <v>481</v>
       </c>
       <c r="D2">
         <v>15000000</v>
@@ -3450,31 +3399,31 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:P6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.1796875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
     <col min="3" max="3" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
     <col min="4" max="5" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="13.26953125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="12.7265625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="14.453125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="13.28515625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="14.42578125" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="17.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3515,82 +3464,82 @@
         <v>394</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>402</v>
       </c>
       <c r="B2" t="s">
-        <v>453</v>
+        <v>481</v>
       </c>
       <c r="C2" t="s">
-        <v>454</v>
+        <v>442</v>
       </c>
       <c r="D2" t="s">
-        <v>423</v>
+        <v>468</v>
       </c>
       <c r="E2" t="s">
-        <v>440</v>
+        <v>429</v>
       </c>
       <c r="F2" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
       <c r="G2" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
       <c r="H2" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
       <c r="I2" t="s">
-        <v>442</v>
+        <v>431</v>
       </c>
       <c r="J2" t="s">
-        <v>443</v>
-      </c>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.35">
+        <v>432</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>403</v>
       </c>
       <c r="B3" t="s">
-        <v>453</v>
+        <v>481</v>
       </c>
       <c r="C3" t="s">
-        <v>455</v>
+        <v>443</v>
       </c>
       <c r="D3" t="s">
-        <v>424</v>
+        <v>471</v>
       </c>
       <c r="E3" t="s">
-        <v>441</v>
+        <v>430</v>
       </c>
       <c r="F3" t="s">
         <v>378</v>
       </c>
       <c r="G3" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="H3" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="I3" t="s">
-        <v>444</v>
+        <v>433</v>
       </c>
       <c r="J3" t="s">
-        <v>445</v>
-      </c>
-    </row>
-    <row r="4" spans="1:15" x14ac:dyDescent="0.35">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>404</v>
       </c>
       <c r="B4" t="s">
-        <v>453</v>
+        <v>481</v>
       </c>
       <c r="C4" t="s">
-        <v>456</v>
+        <v>482</v>
       </c>
       <c r="D4" t="s">
-        <v>428</v>
+        <v>463</v>
       </c>
       <c r="E4" t="s">
         <v>420</v>
@@ -3599,105 +3548,105 @@
         <v>409</v>
       </c>
       <c r="G4" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
       <c r="H4" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
       <c r="I4" t="s">
-        <v>446</v>
+        <v>435</v>
       </c>
       <c r="J4" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>405</v>
       </c>
       <c r="B5" t="s">
-        <v>453</v>
+        <v>481</v>
       </c>
       <c r="C5" t="s">
-        <v>457</v>
+        <v>483</v>
       </c>
       <c r="D5" t="s">
-        <v>422</v>
+        <v>464</v>
       </c>
       <c r="E5" t="s">
-        <v>447</v>
+        <v>421</v>
       </c>
       <c r="F5" t="s">
-        <v>448</v>
+        <v>375</v>
       </c>
       <c r="G5" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="H5" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="I5" t="s">
-        <v>449</v>
+        <v>440</v>
       </c>
       <c r="J5" t="s">
-        <v>450</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.35">
+        <v>441</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>406</v>
       </c>
       <c r="B6" t="s">
-        <v>453</v>
+        <v>481</v>
       </c>
       <c r="C6" t="s">
-        <v>458</v>
+        <v>484</v>
       </c>
       <c r="D6" t="s">
-        <v>429</v>
+        <v>467</v>
       </c>
       <c r="E6" t="s">
-        <v>421</v>
+        <v>436</v>
       </c>
       <c r="F6" t="s">
-        <v>375</v>
+        <v>437</v>
       </c>
       <c r="G6" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
       <c r="H6" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
       <c r="I6" t="s">
-        <v>451</v>
+        <v>438</v>
       </c>
       <c r="J6" t="s">
-        <v>452</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="17.453125" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="34.7265625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="36.54296875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="9.7265625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="34.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="36.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="9.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="1" s="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -3714,7 +3663,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>203</v>
       </c>
@@ -3722,7 +3671,7 @@
         <v>204</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>205</v>
       </c>
@@ -3730,13 +3679,13 @@
         <v>206</v>
       </c>
       <c r="C3" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="D3" t="s">
         <v>207</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>208</v>
       </c>
@@ -3747,10 +3696,10 @@
         <v>210</v>
       </c>
       <c r="E4" t="s">
-        <v>427</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>232</v>
       </c>
@@ -3758,7 +3707,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>234</v>
       </c>
@@ -3766,13 +3715,13 @@
         <v>235</v>
       </c>
       <c r="C6" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
       <c r="D6" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>237</v>
       </c>
@@ -3783,31 +3732,31 @@
         <v>239</v>
       </c>
       <c r="E7" t="s">
-        <v>427</v>
+        <v>422</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J3"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView topLeftCell="D1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G2" sqref="G2"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="G2" pane="bottomLeft" sqref="G2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="19" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="19" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="4" width="19.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="37.453125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="37.42578125" collapsed="true"/>
     <col min="6" max="16384" width="19.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3839,7 +3788,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>13</v>
       </c>
@@ -3862,7 +3811,7 @@
         <v>336</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>12</v>
       </c>
@@ -3873,10 +3822,10 @@
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>472</v>
+        <v>448</v>
       </c>
       <c r="E3" t="s">
-        <v>473</v>
+        <v>449</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -3893,40 +3842,40 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="Q14" r:id="rId1" display="www.facebook.com"/>
-    <hyperlink ref="R14" r:id="rId2" display="www.linkedin.com"/>
-    <hyperlink ref="Q15" r:id="rId3" display="www.facebook.com"/>
-    <hyperlink ref="R15" r:id="rId4" display="www.linkedin.com"/>
-    <hyperlink ref="Q3" r:id="rId5" display="www.facebook.com"/>
-    <hyperlink ref="R3" r:id="rId6" display="www.linkedin.com"/>
+    <hyperlink display="www.facebook.com" r:id="rId1" ref="Q14"/>
+    <hyperlink display="www.linkedin.com" r:id="rId2" ref="R14"/>
+    <hyperlink display="www.facebook.com" r:id="rId3" ref="Q15"/>
+    <hyperlink display="www.linkedin.com" r:id="rId4" ref="R15"/>
+    <hyperlink display="www.facebook.com" r:id="rId5" ref="Q3"/>
+    <hyperlink display="www.linkedin.com" r:id="rId6" ref="R3"/>
   </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId7"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="200" orientation="portrait" r:id="rId7" verticalDpi="200"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.0" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="28.26953125" collapsed="true"/>
-    <col min="3" max="3" customWidth="true" width="28.26953125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="29.1796875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="9.453125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="16.54296875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="23.54296875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="19.81640625" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="17.7265625" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" width="28.28515625" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="9.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -3955,15 +3904,15 @@
         <v>125</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35">
+    <row customHeight="1" ht="15" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>478</v>
+        <v>454</v>
       </c>
       <c r="C2" t="s">
-        <v>479</v>
+        <v>455</v>
       </c>
       <c r="D2" t="s">
         <v>110</v>
@@ -3984,32 +3933,32 @@
         <v>117</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.35"/>
+    <row customHeight="1" ht="15" r="6" spans="1:9" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.54296875" collapsed="true"/>
-    <col min="3" max="4" bestFit="true" customWidth="true" width="21.453125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="16.54296875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="29.1796875" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="19.81640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="17.7265625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.5703125" collapsed="true"/>
+    <col min="3" max="4" bestFit="true" customWidth="true" width="21.42578125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="29.140625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="19.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4032,52 +3981,52 @@
       <c r="H1" s="5"/>
       <c r="I1" s="5"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>476</v>
+        <v>485</v>
       </c>
       <c r="C2" t="s">
-        <v>477</v>
+        <v>486</v>
       </c>
       <c r="D2" t="s">
-        <v>474</v>
+        <v>450</v>
       </c>
       <c r="E2" t="s">
-        <v>475</v>
+        <v>451</v>
       </c>
       <c r="F2" t="s">
         <v>122</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X6"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Y6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D13" sqref="D13"/>
+    <sheetView workbookViewId="0">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="D13" pane="bottomLeft" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="22.54296875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="21.81640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="11.54296875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="33.1796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="24.81640625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="21.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="11.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="33.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="24.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="1" s="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4097,7 +4046,7 @@
         <v>309</v>
       </c>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>246</v>
       </c>
@@ -4117,7 +4066,7 @@
         <v>248</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>249</v>
       </c>
@@ -4135,7 +4084,7 @@
       </c>
       <c r="X3" s="27"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>251</v>
       </c>
@@ -4153,7 +4102,7 @@
       </c>
       <c r="X4" s="27"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>254</v>
       </c>
@@ -4171,7 +4120,7 @@
       </c>
       <c r="X5" s="27"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>256</v>
       </c>
@@ -4190,31 +4139,31 @@
   <mergeCells count="1">
     <mergeCell ref="X2:X6"/>
   </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H9"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:K9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="22.26953125" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="31.81640625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="18.1796875" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7265625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="14.7265625" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="13.7265625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="22.81640625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="22.28515625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="14.7109375" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4239,8 +4188,14 @@
       <c r="H1" s="5" t="s">
         <v>220</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="I1" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="J1" s="5" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>221</v>
       </c>
@@ -4265,8 +4220,11 @@
       <c r="H2" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>222</v>
       </c>
@@ -4288,8 +4246,11 @@
       <c r="H3" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J3" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>224</v>
       </c>
@@ -4312,7 +4273,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>226</v>
       </c>
@@ -4334,8 +4295,11 @@
       <c r="H5" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J5" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>227</v>
       </c>
@@ -4358,7 +4322,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>242</v>
       </c>
@@ -4380,8 +4344,11 @@
       <c r="H7" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J7" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>243</v>
       </c>
@@ -4403,8 +4370,11 @@
       <c r="H8" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="J8" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>244</v>
       </c>
@@ -4428,61 +4398,66 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <hyperlinks>
+    <hyperlink display="mailto:navatariptesting+49277@gmail.com" r:id="rId1" ref="J3"/>
+    <hyperlink display="mailto:navatariptesting+49277@gmail.com" r:id="rId2" ref="J5"/>
+    <hyperlink display="mailto:navatariptesting+49277@gmail.com" r:id="rId3" ref="J8"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AL11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" mc:Ignorable="x14ac">
+  <dimension ref="A1:AM11"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="W1" sqref="W1"/>
+    <sheetView topLeftCell="L1" workbookViewId="0">
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="L7" pane="bottomLeft" sqref="L7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="18.1796875" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.7265625" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="19.7265625" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="37.453125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="26.26953125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="26.1796875" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="19.1796875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="18.140625" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.7109375" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="37.42578125" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="26.140625" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="19.140625" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="19.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="12.7265625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="14.54296875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="27.26953125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="14.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="27.28515625" collapsed="true"/>
     <col min="13" max="13" bestFit="true" customWidth="true" width="22.0" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="26.453125" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="27.7265625" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="27.7109375" collapsed="true"/>
     <col min="16" max="16" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="17" max="17" bestFit="true" customWidth="true" width="13.7265625" collapsed="true"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" width="23.1796875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" width="13.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" width="23.140625" collapsed="true"/>
     <col min="19" max="19" bestFit="true" customWidth="true" width="28.0" collapsed="true"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" width="29.453125" collapsed="true"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" width="27.453125" collapsed="true"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" width="25.1796875" collapsed="true"/>
-    <col min="23" max="24" customWidth="true" width="19.7265625" collapsed="true"/>
-    <col min="25" max="25" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
-    <col min="26" max="26" bestFit="true" customWidth="true" width="16.1796875" collapsed="true"/>
-    <col min="27" max="27" width="9.1796875" collapsed="true"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" width="26.453125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" width="29.42578125" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" width="27.42578125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" width="25.140625" collapsed="true"/>
+    <col min="23" max="24" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="27" max="27" width="9.140625" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
     <col min="29" max="29" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="30" max="30" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
-    <col min="31" max="31" bestFit="true" customWidth="true" width="16.1796875" collapsed="true"/>
-    <col min="33" max="33" bestFit="true" customWidth="true" width="26.453125" collapsed="true"/>
+    <col min="30" max="30" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="31" max="31" bestFit="true" customWidth="true" width="16.140625" collapsed="true"/>
+    <col min="33" max="33" bestFit="true" customWidth="true" width="26.42578125" collapsed="true"/>
     <col min="34" max="34" bestFit="true" customWidth="true" width="21.0" collapsed="true"/>
-    <col min="35" max="35" customWidth="true" width="14.453125" collapsed="true"/>
-    <col min="36" max="36" customWidth="true" width="15.54296875" collapsed="true"/>
+    <col min="35" max="35" customWidth="true" width="14.42578125" collapsed="true"/>
+    <col min="36" max="36" customWidth="true" width="15.5703125" collapsed="true"/>
     <col min="37" max="37" customWidth="true" style="6" width="15.0" collapsed="true"/>
-    <col min="38" max="38" bestFit="true" customWidth="true" width="30.453125" collapsed="true"/>
-    <col min="39" max="39" bestFit="true" customWidth="true" width="22.54296875" collapsed="true"/>
+    <col min="38" max="38" bestFit="true" customWidth="true" width="30.42578125" collapsed="true"/>
+    <col min="39" max="39" bestFit="true" customWidth="true" width="22.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="1" s="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4554,7 +4529,7 @@
       </c>
       <c r="AL1" s="3"/>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>101</v>
       </c>
@@ -4567,11 +4542,11 @@
       <c r="D2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
-        <v>482</v>
-      </c>
-    </row>
-    <row r="3" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="E2" s="2" t="s">
+        <v>457</v>
+      </c>
+    </row>
+    <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>102</v>
       </c>
@@ -4584,11 +4559,11 @@
       <c r="D3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" t="s">
-        <v>483</v>
-      </c>
-    </row>
-    <row r="4" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="E3" s="2" t="s">
+        <v>456</v>
+      </c>
+    </row>
+    <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>103</v>
       </c>
@@ -4601,11 +4576,11 @@
       <c r="D4" t="s">
         <v>36</v>
       </c>
-      <c r="E4" t="s">
-        <v>484</v>
-      </c>
-    </row>
-    <row r="5" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="E4" s="2" t="s">
+        <v>458</v>
+      </c>
+    </row>
+    <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>104</v>
       </c>
@@ -4619,7 +4594,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>105</v>
       </c>
@@ -4632,11 +4607,11 @@
       <c r="D6" t="s">
         <v>41</v>
       </c>
-      <c r="E6" t="s">
-        <v>480</v>
-      </c>
-    </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.35">
+      <c r="E6" s="2" t="s">
+        <v>459</v>
+      </c>
+    </row>
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>106</v>
       </c>
@@ -4649,8 +4624,8 @@
       <c r="D7" t="s">
         <v>48</v>
       </c>
-      <c r="E7" t="s">
-        <v>481</v>
+      <c r="E7" s="2" t="s">
+        <v>460</v>
       </c>
       <c r="L7" t="s">
         <v>67</v>
@@ -4668,7 +4643,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>351</v>
       </c>
@@ -4682,7 +4657,7 @@
         <v>314</v>
       </c>
       <c r="E8" t="s">
-        <v>470</v>
+        <v>446</v>
       </c>
       <c r="F8" t="s">
         <v>315</v>
@@ -4735,7 +4710,7 @@
       <c r="AJ8" s="6"/>
       <c r="AK8"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>352</v>
       </c>
@@ -4799,7 +4774,7 @@
       <c r="AJ9" s="6"/>
       <c r="AK9"/>
     </row>
-    <row r="10" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>353</v>
       </c>
@@ -4863,7 +4838,7 @@
       <c r="AJ10" s="6"/>
       <c r="AK10"/>
     </row>
-    <row r="11" spans="1:38" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>354</v>
       </c>
@@ -4877,7 +4852,7 @@
         <v>334</v>
       </c>
       <c r="E11" t="s">
-        <v>471</v>
+        <v>447</v>
       </c>
       <c r="F11" t="s">
         <v>336</v>
@@ -4934,38 +4909,45 @@
       <c r="AK11"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <hyperlinks>
+    <hyperlink display="mailto:navatariptesting+84488@gmail.com" r:id="rId1" ref="E3"/>
+    <hyperlink r:id="rId2" ref="E2"/>
+    <hyperlink display="mailto:navatariptesting+49277@gmail.com" r:id="rId3" ref="E4"/>
+    <hyperlink display="mailto:navatariptesting+54430@gmail.com" r:id="rId4" ref="E6"/>
+    <hyperlink display="mailto:navatariptesting+40025@gmail.com" r:id="rId5" ref="E7"/>
+  </hyperlinks>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="200" orientation="portrait" r:id="rId6" verticalDpi="200"/>
+  <legacyDrawing r:id="rId7"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:I4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="F2" pane="bottomLeft" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="15.81640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="41.54296875" collapsed="true"/>
-    <col min="5" max="5" customWidth="true" width="24.81640625" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="23" width="19.26953125" collapsed="true"/>
-    <col min="7" max="7" customWidth="true" width="24.81640625" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" style="10" width="24.26953125" collapsed="true"/>
-    <col min="9" max="9" bestFit="true" customWidth="true" width="15.1796875" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="16.7265625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="15.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="41.5703125" collapsed="true"/>
+    <col min="5" max="5" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="23" width="19.28515625" collapsed="true"/>
+    <col min="7" max="7" customWidth="true" width="24.85546875" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="10" width="24.28515625" collapsed="true"/>
+    <col min="9" max="9" bestFit="true" customWidth="true" width="15.140625" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="16.7109375" collapsed="true"/>
     <col min="11" max="11" bestFit="true" customWidth="true" width="36.0" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="37.54296875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="37.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -4991,7 +4973,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>129</v>
       </c>
@@ -5008,16 +4990,16 @@
         <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>495</v>
+        <v>469</v>
       </c>
       <c r="G2">
         <v>2019</v>
       </c>
       <c r="H2" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>130</v>
       </c>
@@ -5040,10 +5022,10 @@
         <v>2020</v>
       </c>
       <c r="H3" t="s">
-        <v>485</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+        <v>452</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>131</v>
       </c>
@@ -5060,42 +5042,42 @@
         <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>501</v>
+        <v>474</v>
       </c>
       <c r="G4">
         <v>2021</v>
       </c>
       <c r="H4" t="s">
-        <v>485</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="200" orientation="portrait" r:id="rId1" verticalDpi="200"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G7"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:H7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F2" sqref="F2"/>
+      <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
+      <selection activeCell="F2" pane="bottomLeft" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="31.81640625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="12.81640625" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="31.85546875" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="12.85546875" collapsed="true"/>
     <col min="4" max="4" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="31.26953125" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="26.26953125" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.7265625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="31.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="26.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.7109375" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -5118,7 +5100,7 @@
         <v>170</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>215</v>
       </c>
@@ -5138,7 +5120,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>218</v>
       </c>
@@ -5158,7 +5140,7 @@
         <v>219</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>228</v>
       </c>
@@ -5181,7 +5163,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>231</v>
       </c>
@@ -5204,7 +5186,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>240</v>
       </c>
@@ -5224,7 +5206,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>241</v>
       </c>
@@ -5245,25 +5227,25 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="22.1796875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="22.140625" collapsed="true"/>
     <col min="2" max="2" bestFit="true" customWidth="true" width="26.0" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>0</v>
       </c>
@@ -5271,7 +5253,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>144</v>
       </c>
@@ -5279,7 +5261,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>145</v>
       </c>
@@ -5287,7 +5269,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>146</v>
       </c>
@@ -5296,39 +5278,39 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:Q4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" width="14.81640625" collapsed="true"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" width="23.7265625" collapsed="true"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" width="17.453125" collapsed="true"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" width="24.26953125" collapsed="true"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" width="24.1796875" collapsed="true"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" width="22.81640625" collapsed="true"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" width="15.453125" collapsed="true"/>
-    <col min="8" max="8" bestFit="true" customWidth="true" width="7.54296875" collapsed="true"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" width="14.85546875" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" width="23.7109375" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" width="17.42578125" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" width="24.28515625" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" width="24.140625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" width="22.85546875" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" width="15.42578125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" width="7.5703125" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="10" max="10" bestFit="true" customWidth="true" width="18.7265625" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="11.81640625" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7265625" collapsed="true"/>
-    <col min="13" max="13" bestFit="true" customWidth="true" width="19.54296875" collapsed="true"/>
-    <col min="14" max="14" bestFit="true" customWidth="true" width="15.54296875" collapsed="true"/>
-    <col min="15" max="15" bestFit="true" customWidth="true" width="19.7265625" collapsed="true"/>
-    <col min="16" max="16" bestFit="true" customWidth="true" width="22.453125" collapsed="true"/>
+    <col min="10" max="10" bestFit="true" customWidth="true" width="18.7109375" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="11.85546875" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="10.7109375" collapsed="true"/>
+    <col min="13" max="13" bestFit="true" customWidth="true" width="19.5703125" collapsed="true"/>
+    <col min="14" max="14" bestFit="true" customWidth="true" width="15.5703125" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" width="19.7109375" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" width="22.42578125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="1" s="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -5378,12 +5360,12 @@
         <v>178</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>504</v>
+        <v>453</v>
       </c>
       <c r="C2" t="s">
         <v>152</v>
@@ -5416,12 +5398,12 @@
         <v>180</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>157</v>
       </c>
       <c r="B3" t="s">
-        <v>468</v>
+        <v>444</v>
       </c>
       <c r="C3" t="s">
         <v>158</v>
@@ -5454,12 +5436,12 @@
         <v>168</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>163</v>
       </c>
       <c r="B4" t="s">
-        <v>469</v>
+        <v>445</v>
       </c>
       <c r="C4" t="s">
         <v>164</v>
@@ -5478,35 +5460,35 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageSetup horizontalDpi="200" orientation="portrait" r:id="rId1" verticalDpi="200"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" bestFit="true" customWidth="true" width="15.0" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" width="29.54296875" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" width="29.5703125" collapsed="true"/>
     <col min="3" max="3" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="4" max="4" customWidth="true" width="12.1796875" collapsed="true"/>
+    <col min="4" max="4" customWidth="true" width="12.140625" collapsed="true"/>
     <col min="5" max="5" customWidth="true" width="18.0" collapsed="true"/>
-    <col min="6" max="6" customWidth="true" width="12.7265625" collapsed="true"/>
-    <col min="8" max="8" customWidth="true" width="20.7265625" collapsed="true"/>
+    <col min="6" max="6" customWidth="true" width="12.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" width="20.7109375" collapsed="true"/>
     <col min="9" max="9" bestFit="true" customWidth="true" width="10.0" collapsed="true"/>
     <col min="10" max="10" bestFit="true" customWidth="true" width="9.0" collapsed="true"/>
-    <col min="11" max="11" bestFit="true" customWidth="true" width="10.54296875" collapsed="true"/>
-    <col min="12" max="12" bestFit="true" customWidth="true" width="16.54296875" collapsed="true"/>
+    <col min="11" max="11" bestFit="true" customWidth="true" width="10.5703125" collapsed="true"/>
+    <col min="12" max="12" bestFit="true" customWidth="true" width="16.5703125" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="1" customFormat="1" x14ac:dyDescent="0.35">
+    <row customFormat="1" r="1" s="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -5544,7 +5526,7 @@
         <v>225</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>185</v>
       </c>
@@ -5582,7 +5564,7 @@
         <v>196</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>191</v>
       </c>
@@ -5620,7 +5602,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>197</v>
       </c>
@@ -5656,6 +5638,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Acutiy 1.0 related changes
Signed-off-by: ravi <rkumar1@navatargroup.com>
</commit_message>
<xml_diff>
--- a/SmokeTestCases.xlsx
+++ b/SmokeTestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView activeTab="18" firstSheet="13" tabRatio="622" windowHeight="11160" windowWidth="20730" xWindow="-120" yWindow="-120"/>
+    <workbookView tabRatio="622" windowHeight="11160" windowWidth="20730" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Institutions" r:id="rId1" sheetId="22"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="487">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="512">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -184,9 +184,6 @@
     <t>TestM1Institution2</t>
   </si>
   <si>
-    <t>Individual Investor</t>
-  </si>
-  <si>
     <t>TestM1Company1</t>
   </si>
   <si>
@@ -1435,27 +1432,12 @@
     <t>TestCompany1 - Feb 2022</t>
   </si>
   <si>
-    <t>PETestEmailFolder90700</t>
-  </si>
-  <si>
-    <t>PETestCustomEmailTemplate25516</t>
-  </si>
-  <si>
-    <t>navatariptesting+84488@gmail.com</t>
-  </si>
-  <si>
     <t>navatariptesting+14032@gmail.com</t>
   </si>
   <si>
     <t>navatariptesting+49277@gmail.com</t>
   </si>
   <si>
-    <t>navatariptesting+54430@gmail.com</t>
-  </si>
-  <si>
-    <t>navatariptesting+40025@gmail.com</t>
-  </si>
-  <si>
     <t>7/20/2022</t>
   </si>
   <si>
@@ -1528,10 +1510,103 @@
     <t>ID-0632</t>
   </si>
   <si>
-    <t>CustomReportFolder47527</t>
-  </si>
-  <si>
-    <t>CustomReport57424</t>
+    <t>CustomReportFolder34737</t>
+  </si>
+  <si>
+    <t>CustomReport44208</t>
+  </si>
+  <si>
+    <t>PETestEmailFolder47379</t>
+  </si>
+  <si>
+    <t>PETestCustomEmailTemplate59619</t>
+  </si>
+  <si>
+    <t>navatariptesting+93803@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+66562@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+8075@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+11803@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+19040@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+20511@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+29440@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+37761@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+10459@gmail.com</t>
+  </si>
+  <si>
+    <t>9/20/2022</t>
+  </si>
+  <si>
+    <t>navatariptesting+38840@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+91042@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+94321@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+52197@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+4134@gmail.com</t>
+  </si>
+  <si>
+    <t>6.3E8</t>
+  </si>
+  <si>
+    <t>9/21/2022</t>
+  </si>
+  <si>
+    <t>9/22/2022</t>
+  </si>
+  <si>
+    <t>CMT - 000950</t>
+  </si>
+  <si>
+    <t>CMT - 000951</t>
+  </si>
+  <si>
+    <t>6.7E8</t>
+  </si>
+  <si>
+    <t>9/24/2022</t>
+  </si>
+  <si>
+    <t>9/25/2022</t>
+  </si>
+  <si>
+    <t>6.75E8</t>
+  </si>
+  <si>
+    <t>9/28/2022</t>
+  </si>
+  <si>
+    <t>7.2E7</t>
+  </si>
+  <si>
+    <t>10/1/2022</t>
+  </si>
+  <si>
+    <t>8.4E7</t>
+  </si>
+  <si>
+    <t>10/6/2022</t>
   </si>
 </sst>
 </file>
@@ -1958,9 +2033,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="A9" pane="bottomLeft" sqref="A9"/>
+      <selection activeCell="B13" pane="bottomLeft" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2000,10 +2075,10 @@
         <v>29</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>30</v>
@@ -2015,43 +2090,43 @@
         <v>32</v>
       </c>
       <c r="I1" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="J1" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="K1" s="7" t="s">
+        <v>355</v>
+      </c>
+      <c r="L1" s="7" t="s">
+        <v>132</v>
+      </c>
+      <c r="M1" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="N1" s="7" t="s">
+        <v>58</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="S1" s="7" t="s">
         <v>56</v>
       </c>
-      <c r="K1" s="7" t="s">
-        <v>356</v>
-      </c>
-      <c r="L1" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="M1" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="N1" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="O1" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>137</v>
-      </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>57</v>
       </c>
-      <c r="T1" s="7" t="s">
-        <v>58</v>
-      </c>
       <c r="U1" s="7" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>26</v>
@@ -2062,7 +2137,7 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
@@ -2073,28 +2148,28 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>
       </c>
       <c r="L3" t="s">
+        <v>41</v>
+      </c>
+      <c r="M3" t="s">
         <v>42</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>43</v>
-      </c>
-      <c r="N3" t="s">
-        <v>44</v>
       </c>
       <c r="O3">
         <v>210310</v>
       </c>
       <c r="P3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V3">
         <v>3636366336</v>
@@ -2105,10 +2180,10 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -2116,28 +2191,28 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
       </c>
       <c r="L5" t="s">
+        <v>48</v>
+      </c>
+      <c r="M5" t="s">
         <v>49</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>50</v>
-      </c>
-      <c r="N5" t="s">
-        <v>51</v>
       </c>
       <c r="O5">
         <v>900268</v>
       </c>
       <c r="P5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="V5">
         <v>66228811</v>
@@ -2148,10 +2223,10 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C6" t="s">
         <v>35</v>
@@ -2159,169 +2234,169 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B7" t="s">
         <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C8" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B9" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B10" t="s">
+        <v>37</v>
+      </c>
+      <c r="C10" t="s">
         <v>38</v>
-      </c>
-      <c r="C10" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B11" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C11" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="B12" t="s">
+        <v>313</v>
+      </c>
+      <c r="C12" t="s">
+        <v>35</v>
+      </c>
+      <c r="H12" t="s">
         <v>314</v>
       </c>
-      <c r="C12" t="s">
-        <v>37</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>315</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>316</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>317</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>318</v>
       </c>
-      <c r="L12" t="s">
-        <v>319</v>
-      </c>
       <c r="M12" t="s">
+        <v>42</v>
+      </c>
+      <c r="N12" t="s">
         <v>43</v>
-      </c>
-      <c r="N12" t="s">
-        <v>44</v>
       </c>
       <c r="O12">
         <v>281001</v>
       </c>
       <c r="P12" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q12" t="s">
+        <v>319</v>
+      </c>
+      <c r="R12" t="s">
         <v>320</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>321</v>
-      </c>
-      <c r="S12" t="s">
-        <v>322</v>
       </c>
       <c r="T12">
         <v>200300</v>
       </c>
       <c r="U12" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="V12">
         <v>2121212121</v>
       </c>
       <c r="W12" s="15" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="B13" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C13" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H13" t="s">
+        <v>323</v>
+      </c>
+      <c r="I13" t="s">
+        <v>315</v>
+      </c>
+      <c r="J13" t="s">
+        <v>316</v>
+      </c>
+      <c r="K13" t="s">
+        <v>317</v>
+      </c>
+      <c r="L13" t="s">
         <v>324</v>
       </c>
-      <c r="I13" t="s">
-        <v>316</v>
-      </c>
-      <c r="J13" t="s">
-        <v>317</v>
-      </c>
-      <c r="K13" t="s">
-        <v>318</v>
-      </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>325</v>
       </c>
-      <c r="M13" t="s">
-        <v>326</v>
-      </c>
       <c r="N13" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O13">
         <v>201301</v>
       </c>
       <c r="P13" t="s">
+        <v>326</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>369</v>
+      </c>
+      <c r="R13" t="s">
         <v>327</v>
       </c>
-      <c r="Q13" t="s">
-        <v>370</v>
-      </c>
-      <c r="R13" t="s">
-        <v>328</v>
-      </c>
       <c r="S13" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="T13">
         <v>10016</v>
       </c>
       <c r="U13" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="V13">
         <v>98765429</v>
@@ -2329,55 +2404,55 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="B14" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="C14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="H14" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I14" t="s">
+        <v>315</v>
+      </c>
+      <c r="J14" t="s">
         <v>316</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>317</v>
       </c>
-      <c r="K14" t="s">
-        <v>318</v>
-      </c>
       <c r="L14" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="M14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="N14" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="O14">
         <v>500700</v>
       </c>
       <c r="P14" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="Q14" t="s">
+        <v>330</v>
+      </c>
+      <c r="R14" t="s">
         <v>331</v>
       </c>
-      <c r="R14" t="s">
-        <v>332</v>
-      </c>
       <c r="S14" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="T14">
         <v>2834</v>
       </c>
       <c r="U14" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="V14">
         <v>1629539588</v>
@@ -2385,58 +2460,58 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="B15" t="s">
+        <v>333</v>
+      </c>
+      <c r="C15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="2" t="s">
         <v>334</v>
       </c>
-      <c r="C15" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="2" t="s">
+      <c r="H15" t="s">
         <v>335</v>
       </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
+        <v>315</v>
+      </c>
+      <c r="J15" t="s">
         <v>336</v>
       </c>
-      <c r="I15" t="s">
-        <v>316</v>
-      </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>337</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>338</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
+        <v>386</v>
+      </c>
+      <c r="N15" t="s">
         <v>339</v>
-      </c>
-      <c r="M15" t="s">
-        <v>387</v>
-      </c>
-      <c r="N15" t="s">
-        <v>340</v>
       </c>
       <c r="O15">
         <v>560003</v>
       </c>
       <c r="P15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q15" t="s">
+        <v>338</v>
+      </c>
+      <c r="R15" t="s">
+        <v>386</v>
+      </c>
+      <c r="S15" t="s">
         <v>339</v>
-      </c>
-      <c r="R15" t="s">
-        <v>387</v>
-      </c>
-      <c r="S15" t="s">
-        <v>340</v>
       </c>
       <c r="T15">
         <v>560003</v>
       </c>
       <c r="U15" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="V15">
         <v>9999999999</v>
@@ -2479,54 +2554,54 @@
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>259</v>
+      </c>
+      <c r="B2" t="s">
         <v>260</v>
       </c>
-      <c r="B2" t="s">
-        <v>261</v>
-      </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>261</v>
+      </c>
+      <c r="B3" t="s">
         <v>262</v>
       </c>
-      <c r="B3" t="s">
-        <v>263</v>
-      </c>
       <c r="C3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D3" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>263</v>
+      </c>
+      <c r="B4" t="s">
         <v>264</v>
       </c>
-      <c r="B4" t="s">
-        <v>265</v>
-      </c>
       <c r="C4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>265</v>
+      </c>
+      <c r="B5" t="s">
         <v>266</v>
       </c>
-      <c r="B5" t="s">
-        <v>267</v>
-      </c>
       <c r="C5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>
@@ -2575,135 +2650,135 @@
         <v>21</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>268</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="H1" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>313</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>312</v>
-      </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>270</v>
       </c>
-      <c r="I1" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="19" t="s">
         <v>271</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="L1" s="19" t="s">
         <v>272</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="M1" s="19" t="s">
         <v>273</v>
       </c>
-      <c r="M1" s="19" t="s">
+      <c r="N1" s="19" t="s">
         <v>274</v>
       </c>
-      <c r="N1" s="19" t="s">
+      <c r="O1" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="O1" s="3" t="s">
+      <c r="P1" s="3" t="s">
         <v>276</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="16" t="s">
+        <v>398</v>
+      </c>
+      <c r="R1" s="26" t="s">
+        <v>409</v>
+      </c>
+      <c r="S1" s="16" t="s">
+        <v>410</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>277</v>
-      </c>
-      <c r="Q1" s="16" t="s">
-        <v>399</v>
-      </c>
-      <c r="R1" s="26" t="s">
-        <v>410</v>
-      </c>
-      <c r="S1" s="16" t="s">
-        <v>411</v>
-      </c>
-      <c r="T1" s="3" t="s">
-        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B2" t="s">
-        <v>463</v>
+        <v>501</v>
       </c>
       <c r="C2" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D2" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E2">
         <v>20000000</v>
       </c>
       <c r="F2" t="s">
+        <v>279</v>
+      </c>
+      <c r="G2" t="s">
         <v>280</v>
       </c>
-      <c r="G2" t="s">
-        <v>281</v>
-      </c>
       <c r="H2" t="s">
-        <v>461</v>
+        <v>499</v>
       </c>
       <c r="P2" s="18"/>
       <c r="T2" s="28" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B3" t="s">
-        <v>464</v>
+        <v>502</v>
       </c>
       <c r="C3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="D3" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E3">
         <v>10000000</v>
       </c>
       <c r="F3" t="s">
+        <v>279</v>
+      </c>
+      <c r="G3" t="s">
         <v>280</v>
       </c>
-      <c r="G3" t="s">
-        <v>281</v>
-      </c>
       <c r="H3" t="s">
-        <v>462</v>
+        <v>500</v>
       </c>
       <c r="T3" s="28"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B4" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
       <c r="C4" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D4" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E4">
         <v>15000000</v>
       </c>
       <c r="H4" t="s">
-        <v>465</v>
+        <v>504</v>
       </c>
       <c r="J4">
         <v>7.5</v>
@@ -2712,22 +2787,22 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B5" t="s">
-        <v>468</v>
+        <v>458</v>
       </c>
       <c r="C5" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="D5" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E5">
         <v>25000000</v>
       </c>
       <c r="H5" t="s">
-        <v>466</v>
+        <v>505</v>
       </c>
       <c r="J5">
         <v>7.5</v>
@@ -2736,100 +2811,100 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
       <c r="B6" t="s">
-        <v>471</v>
+        <v>461</v>
       </c>
       <c r="C6" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D6" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="E6">
         <v>5000000</v>
       </c>
       <c r="H6" t="s">
-        <v>470</v>
+        <v>507</v>
       </c>
       <c r="T6" s="28"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
       <c r="B7" t="s">
-        <v>473</v>
+        <v>462</v>
       </c>
       <c r="C7" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="D7" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="E7">
         <v>2000000</v>
       </c>
       <c r="H7" t="s">
-        <v>472</v>
+        <v>509</v>
       </c>
       <c r="I7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T7" s="28"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="B8" t="s">
-        <v>476</v>
+        <v>465</v>
       </c>
       <c r="C8" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="D8" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="E8">
         <v>12000000</v>
       </c>
       <c r="H8" t="s">
-        <v>475</v>
+        <v>511</v>
       </c>
       <c r="I8" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="T8" s="28"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="B9" t="s">
-        <v>463</v>
+        <v>501</v>
       </c>
       <c r="C9" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D9" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E9">
         <v>20000000</v>
       </c>
       <c r="F9" t="s">
+        <v>279</v>
+      </c>
+      <c r="G9" t="s">
         <v>280</v>
       </c>
-      <c r="G9" t="s">
-        <v>281</v>
-      </c>
       <c r="H9" t="s">
-        <v>461</v>
+        <v>499</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="L9" s="14">
         <v>2000000</v>
@@ -2841,48 +2916,48 @@
         <v>0</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="P9" s="14">
         <v>0</v>
       </c>
       <c r="Q9" s="15" t="s">
+        <v>407</v>
+      </c>
+      <c r="R9" s="15" t="s">
         <v>408</v>
-      </c>
-      <c r="R9" s="15" t="s">
-        <v>409</v>
       </c>
       <c r="S9">
         <v>0</v>
       </c>
       <c r="T9" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B10" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="C10" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="D10" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="E10">
         <v>20000000</v>
       </c>
       <c r="F10" t="s">
+        <v>279</v>
+      </c>
+      <c r="G10" t="s">
         <v>280</v>
       </c>
-      <c r="G10" t="s">
-        <v>281</v>
-      </c>
       <c r="H10" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="K10" s="15">
         <v>2000000</v>
@@ -2897,7 +2972,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="P10" s="14">
         <v>0</v>
@@ -2912,7 +2987,7 @@
         <v>0</v>
       </c>
       <c r="T10" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
   </sheetData>
@@ -2951,245 +3026,245 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="19" t="s">
+        <v>293</v>
+      </c>
+      <c r="F1" s="19" t="s">
         <v>294</v>
       </c>
-      <c r="F1" s="19" t="s">
+      <c r="G1" s="19" t="s">
         <v>295</v>
       </c>
-      <c r="G1" s="19" t="s">
+      <c r="H1" s="19" t="s">
         <v>296</v>
       </c>
-      <c r="H1" s="19" t="s">
+      <c r="I1" s="19" t="s">
         <v>297</v>
       </c>
-      <c r="I1" s="19" t="s">
+      <c r="J1" s="19" t="s">
         <v>298</v>
       </c>
-      <c r="J1" s="19" t="s">
+      <c r="K1" s="19" t="s">
         <v>299</v>
       </c>
-      <c r="K1" s="19" t="s">
+      <c r="L1" s="19" t="s">
         <v>300</v>
       </c>
-      <c r="L1" s="19" t="s">
+      <c r="M1" s="19" t="s">
         <v>301</v>
-      </c>
-      <c r="M1" s="19" t="s">
-        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
       <c r="B2" t="s">
-        <v>427</v>
+        <v>426</v>
       </c>
       <c r="C2" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="D2" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E2" t="s">
-        <v>375</v>
+        <v>422</v>
       </c>
       <c r="F2" t="s">
-        <v>382</v>
+        <v>423</v>
       </c>
       <c r="G2" t="s">
-        <v>382</v>
+        <v>423</v>
       </c>
       <c r="H2" t="s">
-        <v>383</v>
+        <v>424</v>
       </c>
       <c r="I2" t="s">
-        <v>461</v>
+        <v>499</v>
       </c>
       <c r="J2" t="s">
-        <v>462</v>
+        <v>500</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="M2" t="s">
-        <v>362</v>
+        <v>425</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
       <c r="B3" t="s">
-        <v>428</v>
+        <v>427</v>
       </c>
       <c r="C3" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="D3" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
       <c r="E3" t="s">
-        <v>423</v>
+        <v>374</v>
       </c>
       <c r="F3" t="s">
-        <v>424</v>
+        <v>381</v>
       </c>
       <c r="G3" t="s">
-        <v>424</v>
+        <v>381</v>
       </c>
       <c r="H3" t="s">
-        <v>425</v>
+        <v>382</v>
       </c>
       <c r="I3" t="s">
-        <v>461</v>
+        <v>499</v>
       </c>
       <c r="J3" t="s">
-        <v>462</v>
+        <v>500</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="M3" t="s">
-        <v>426</v>
+        <v>361</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
       <c r="B4" t="s">
-        <v>478</v>
+        <v>472</v>
       </c>
       <c r="C4" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="D4" t="s">
-        <v>463</v>
+        <v>501</v>
       </c>
       <c r="E4" t="s">
+        <v>372</v>
+      </c>
+      <c r="F4" t="s">
         <v>373</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>373</v>
+      </c>
+      <c r="H4" t="s">
         <v>374</v>
       </c>
-      <c r="G4" t="s">
+      <c r="I4" t="s">
+        <v>499</v>
+      </c>
+      <c r="J4" t="s">
+        <v>500</v>
+      </c>
+      <c r="K4" t="s">
         <v>374</v>
       </c>
-      <c r="H4" t="s">
-        <v>375</v>
-      </c>
-      <c r="I4" t="s">
-        <v>461</v>
-      </c>
-      <c r="J4" t="s">
-        <v>462</v>
-      </c>
-      <c r="K4" t="s">
-        <v>375</v>
-      </c>
       <c r="L4" t="s">
-        <v>461</v>
+        <v>499</v>
       </c>
       <c r="M4" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
       <c r="B5" t="s">
-        <v>479</v>
+        <v>473</v>
       </c>
       <c r="C5" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="D5" t="s">
-        <v>464</v>
+        <v>502</v>
       </c>
       <c r="E5" t="s">
+        <v>375</v>
+      </c>
+      <c r="F5" t="s">
         <v>376</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
+        <v>376</v>
+      </c>
+      <c r="H5" t="s">
         <v>377</v>
       </c>
-      <c r="G5" t="s">
-        <v>377</v>
-      </c>
-      <c r="H5" t="s">
-        <v>378</v>
-      </c>
       <c r="I5" t="s">
-        <v>461</v>
+        <v>499</v>
       </c>
       <c r="J5" t="s">
-        <v>462</v>
+        <v>500</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="M5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
       <c r="B6" t="s">
-        <v>480</v>
+        <v>474</v>
       </c>
       <c r="C6" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="D6" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
       <c r="E6" t="s">
+        <v>378</v>
+      </c>
+      <c r="F6" t="s">
         <v>379</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
+        <v>379</v>
+      </c>
+      <c r="H6" t="s">
         <v>380</v>
       </c>
-      <c r="G6" t="s">
-        <v>380</v>
-      </c>
-      <c r="H6" t="s">
-        <v>381</v>
-      </c>
       <c r="I6" t="s">
-        <v>461</v>
+        <v>499</v>
       </c>
       <c r="J6" t="s">
-        <v>462</v>
+        <v>500</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="M6" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
     </row>
   </sheetData>
@@ -3224,66 +3299,66 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>297</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
         <v>298</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>299</v>
-      </c>
       <c r="G1" s="3" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="I1" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="J1" s="3" t="s">
         <v>294</v>
       </c>
-      <c r="J1" s="3" t="s">
+      <c r="K1" s="3" t="s">
         <v>295</v>
       </c>
-      <c r="K1" s="3" t="s">
-        <v>296</v>
-      </c>
       <c r="L1" s="3" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>390</v>
-      </c>
       <c r="O1" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
       <c r="B2" t="s">
-        <v>477</v>
+        <v>471</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E2" t="s">
-        <v>461</v>
+        <v>499</v>
       </c>
       <c r="F2" t="s">
-        <v>462</v>
+        <v>500</v>
       </c>
       <c r="G2" s="14">
         <v>5500000</v>
@@ -3292,16 +3367,16 @@
         <v>2000000</v>
       </c>
       <c r="I2" s="14" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="J2" s="14" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="K2" s="14">
         <v>750000</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="M2" s="15">
         <v>0</v>
@@ -3342,48 +3417,48 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>299</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="H1" s="3" t="s">
-        <v>295</v>
-      </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>399</v>
-      </c>
       <c r="K1" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="L1" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="L1" s="3" t="s">
-        <v>390</v>
-      </c>
       <c r="M1" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="B2" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="D2">
         <v>15000000</v>
@@ -3428,200 +3503,200 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>400</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>401</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>394</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>395</v>
       </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>396</v>
       </c>
-      <c r="H1" s="3" t="s">
+      <c r="I1" s="3" t="s">
         <v>397</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>398</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>399</v>
-      </c>
       <c r="M1" s="3" t="s">
+        <v>388</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>389</v>
       </c>
-      <c r="N1" s="3" t="s">
-        <v>390</v>
-      </c>
       <c r="O1" s="3" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="B2" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="C2" t="s">
-        <v>442</v>
+        <v>441</v>
       </c>
       <c r="D2" t="s">
-        <v>468</v>
+        <v>461</v>
       </c>
       <c r="E2" t="s">
         <v>429</v>
       </c>
       <c r="F2" t="s">
-        <v>430</v>
+        <v>377</v>
       </c>
       <c r="G2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="H2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="I2" t="s">
-        <v>431</v>
+        <v>432</v>
       </c>
       <c r="J2" t="s">
-        <v>432</v>
+        <v>433</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="B3" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="C3" t="s">
-        <v>443</v>
+        <v>442</v>
       </c>
       <c r="D3" t="s">
-        <v>471</v>
+        <v>458</v>
       </c>
       <c r="E3" t="s">
+        <v>428</v>
+      </c>
+      <c r="F3" t="s">
+        <v>429</v>
+      </c>
+      <c r="G3" t="s">
         <v>430</v>
       </c>
-      <c r="F3" t="s">
-        <v>378</v>
-      </c>
-      <c r="G3" t="s">
-        <v>433</v>
-      </c>
       <c r="H3" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="I3" t="s">
-        <v>433</v>
+        <v>430</v>
       </c>
       <c r="J3" t="s">
-        <v>434</v>
+        <v>431</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="B4" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="C4" t="s">
-        <v>482</v>
+        <v>476</v>
       </c>
       <c r="D4" t="s">
-        <v>463</v>
+        <v>501</v>
       </c>
       <c r="E4" t="s">
-        <v>420</v>
+        <v>419</v>
       </c>
       <c r="F4" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="G4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="H4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="I4" t="s">
-        <v>435</v>
+        <v>434</v>
       </c>
       <c r="J4" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="B5" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="C5" t="s">
-        <v>483</v>
+        <v>477</v>
       </c>
       <c r="D5" t="s">
-        <v>464</v>
+        <v>502</v>
       </c>
       <c r="E5" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="F5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="G5" t="s">
+        <v>439</v>
+      </c>
+      <c r="H5" t="s">
+        <v>439</v>
+      </c>
+      <c r="I5" t="s">
+        <v>439</v>
+      </c>
+      <c r="J5" t="s">
         <v>440</v>
-      </c>
-      <c r="H5" t="s">
-        <v>440</v>
-      </c>
-      <c r="I5" t="s">
-        <v>440</v>
-      </c>
-      <c r="J5" t="s">
-        <v>441</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="B6" t="s">
-        <v>481</v>
+        <v>475</v>
       </c>
       <c r="C6" t="s">
-        <v>484</v>
+        <v>478</v>
       </c>
       <c r="D6" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
       <c r="E6" t="s">
+        <v>435</v>
+      </c>
+      <c r="F6" t="s">
         <v>436</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>437</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
+        <v>437</v>
+      </c>
+      <c r="I6" t="s">
+        <v>437</v>
+      </c>
+      <c r="J6" t="s">
         <v>438</v>
-      </c>
-      <c r="H6" t="s">
-        <v>438</v>
-      </c>
-      <c r="I6" t="s">
-        <v>438</v>
-      </c>
-      <c r="J6" t="s">
-        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -3651,88 +3726,88 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>199</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>200</v>
       </c>
-      <c r="D1" s="3" t="s">
+      <c r="E1" s="3" t="s">
         <v>201</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>202</v>
+      </c>
+      <c r="B2" t="s">
         <v>203</v>
-      </c>
-      <c r="B2" t="s">
-        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>204</v>
+      </c>
+      <c r="B3" t="s">
         <v>205</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
+        <v>421</v>
+      </c>
+      <c r="D3" t="s">
         <v>206</v>
-      </c>
-      <c r="C3" t="s">
-        <v>422</v>
-      </c>
-      <c r="D3" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>207</v>
+      </c>
+      <c r="B4" t="s">
         <v>208</v>
       </c>
-      <c r="B4" t="s">
+      <c r="D4" t="s">
         <v>209</v>
       </c>
-      <c r="D4" t="s">
-        <v>210</v>
-      </c>
       <c r="E4" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>231</v>
+      </c>
+      <c r="B5" t="s">
         <v>232</v>
-      </c>
-      <c r="B5" t="s">
-        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>233</v>
+      </c>
+      <c r="B6" t="s">
         <v>234</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C6" t="s">
+        <v>421</v>
+      </c>
+      <c r="D6" t="s">
         <v>235</v>
-      </c>
-      <c r="C6" t="s">
-        <v>422</v>
-      </c>
-      <c r="D6" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
+        <v>236</v>
+      </c>
+      <c r="B7" t="s">
         <v>237</v>
       </c>
-      <c r="B7" t="s">
+      <c r="D7" t="s">
         <v>238</v>
       </c>
-      <c r="D7" t="s">
-        <v>239</v>
-      </c>
       <c r="E7" t="s">
-        <v>422</v>
+        <v>421</v>
       </c>
     </row>
   </sheetData>
@@ -3785,7 +3860,7 @@
         <v>25</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -3808,7 +3883,7 @@
         <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -3816,16 +3891,16 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="D3" t="s">
+        <v>447</v>
+      </c>
+      <c r="E3" t="s">
         <v>448</v>
-      </c>
-      <c r="E3" t="s">
-        <v>449</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -3834,10 +3909,10 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
+        <v>78</v>
+      </c>
+      <c r="I3" t="s">
         <v>79</v>
-      </c>
-      <c r="I3" t="s">
-        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3880,57 +3955,57 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>112</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C1" s="5" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>109</v>
-      </c>
       <c r="E1" s="5" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>454</v>
+        <v>481</v>
       </c>
       <c r="C2" t="s">
-        <v>455</v>
+        <v>482</v>
       </c>
       <c r="D2" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E2" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="F2" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="H2" t="s">
+        <v>115</v>
+      </c>
+      <c r="I2" t="s">
         <v>116</v>
-      </c>
-      <c r="I2" t="s">
-        <v>117</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="6" spans="1:9" x14ac:dyDescent="0.25"/>
@@ -3943,7 +4018,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -3963,19 +4038,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="F1" s="5" t="s">
         <v>120</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>121</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -3983,22 +4058,22 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>485</v>
+        <v>479</v>
       </c>
       <c r="C2" t="s">
-        <v>486</v>
+        <v>480</v>
       </c>
       <c r="D2" t="s">
+        <v>449</v>
+      </c>
+      <c r="E2" t="s">
         <v>450</v>
       </c>
-      <c r="E2" t="s">
-        <v>451</v>
-      </c>
       <c r="F2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
   </sheetData>
@@ -4034,86 +4109,86 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E1" s="5" t="s">
+        <v>307</v>
+      </c>
+      <c r="F1" s="5" t="s">
         <v>308</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
       </c>
       <c r="C2" t="s">
+        <v>246</v>
+      </c>
+      <c r="E2" s="20" t="s">
+        <v>229</v>
+      </c>
+      <c r="F2" t="s">
+        <v>419</v>
+      </c>
+      <c r="X2" s="27" t="s">
         <v>247</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>230</v>
-      </c>
-      <c r="F2" t="s">
-        <v>420</v>
-      </c>
-      <c r="X2" s="27" t="s">
-        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F3" t="s">
-        <v>421</v>
+        <v>420</v>
       </c>
       <c r="X3" s="27"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
       </c>
       <c r="C4" t="s">
+        <v>251</v>
+      </c>
+      <c r="D4" t="s">
         <v>252</v>
       </c>
-      <c r="D4" t="s">
-        <v>253</v>
-      </c>
       <c r="E4" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="X4" s="27"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="F5">
         <v>5000000</v>
@@ -4122,16 +4197,16 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="X6" s="27"/>
     </row>
@@ -4168,10 +4243,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
@@ -4183,91 +4258,91 @@
         <v>7</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>26</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B2" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="C2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" t="s">
         <v>84</v>
-      </c>
-      <c r="G2" t="s">
-        <v>85</v>
       </c>
       <c r="H2" t="s">
         <v>34</v>
       </c>
       <c r="J2" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B3" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G3" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H3" t="s">
         <v>36</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B4" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="C4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G4" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H4" t="s">
         <v>36</v>
@@ -4275,48 +4350,48 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B5" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="C5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G5" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H5" t="s">
         <v>36</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B6" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="C6" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G6" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H6" t="s">
         <v>36</v>
@@ -4324,74 +4399,74 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B7" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="C7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G7" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H7" t="s">
         <v>34</v>
       </c>
       <c r="J7" t="s">
-        <v>457</v>
+        <v>453</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B8" t="s">
-        <v>418</v>
+        <v>417</v>
       </c>
       <c r="C8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="G8" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H8" t="s">
         <v>36</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>458</v>
+        <v>454</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B9" t="s">
-        <v>419</v>
+        <v>418</v>
       </c>
       <c r="C9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="G9" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="H9" t="s">
         <v>36</v>
@@ -4486,43 +4561,43 @@
         <v>28</v>
       </c>
       <c r="J1" s="5" t="s">
+        <v>137</v>
+      </c>
+      <c r="K1" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="K1" s="5" t="s">
+      <c r="L1" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="L1" s="5" t="s">
+      <c r="M1" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="M1" s="5" t="s">
+      <c r="N1" s="8" t="s">
+        <v>68</v>
+      </c>
+      <c r="O1" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="P1" s="5" t="s">
         <v>141</v>
       </c>
-      <c r="N1" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="O1" s="8" t="s">
-        <v>70</v>
-      </c>
-      <c r="P1" s="5" t="s">
-        <v>142</v>
-      </c>
       <c r="Q1" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="R1" s="5" t="s">
         <v>33</v>
       </c>
       <c r="S1" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="T1" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="U1" s="5" t="s">
         <v>367</v>
       </c>
-      <c r="T1" s="5" t="s">
-        <v>355</v>
-      </c>
-      <c r="U1" s="5" t="s">
-        <v>368</v>
-      </c>
       <c r="V1" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="W1" s="5" t="s">
         <v>29</v>
@@ -4531,64 +4606,64 @@
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="D2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>457</v>
+      <c r="E2" t="s">
+        <v>495</v>
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="2" t="s">
-        <v>456</v>
+      <c r="E3" t="s">
+        <v>496</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="D4" t="s">
         <v>36</v>
       </c>
-      <c r="E4" s="2" t="s">
-        <v>458</v>
+      <c r="E4" t="s">
+        <v>497</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D5" t="s">
         <v>36</v>
@@ -4596,101 +4671,101 @@
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" s="2" t="s">
-        <v>459</v>
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
+        <v>493</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B7" t="s">
+        <v>64</v>
+      </c>
+      <c r="C7" t="s">
         <v>65</v>
       </c>
-      <c r="C7" t="s">
+      <c r="D7" t="s">
+        <v>47</v>
+      </c>
+      <c r="E7" t="s">
+        <v>494</v>
+      </c>
+      <c r="L7" t="s">
         <v>66</v>
       </c>
-      <c r="D7" t="s">
-        <v>48</v>
-      </c>
-      <c r="E7" s="2" t="s">
-        <v>460</v>
-      </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>67</v>
       </c>
-      <c r="M7" t="s">
-        <v>68</v>
-      </c>
       <c r="N7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="O7">
         <v>654927</v>
       </c>
       <c r="P7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="B8" t="s">
+        <v>344</v>
+      </c>
+      <c r="C8" t="s">
         <v>345</v>
       </c>
-      <c r="C8" t="s">
-        <v>346</v>
-      </c>
       <c r="D8" t="s">
+        <v>313</v>
+      </c>
+      <c r="E8" t="s">
+        <v>445</v>
+      </c>
+      <c r="F8" t="s">
         <v>314</v>
       </c>
-      <c r="E8" t="s">
-        <v>446</v>
-      </c>
-      <c r="F8" t="s">
-        <v>315</v>
-      </c>
       <c r="G8" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="H8" t="s">
+        <v>42</v>
+      </c>
+      <c r="I8" t="s">
         <v>43</v>
-      </c>
-      <c r="I8" t="s">
-        <v>44</v>
       </c>
       <c r="J8">
         <v>281001</v>
       </c>
       <c r="K8" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L8" t="s">
+        <v>319</v>
+      </c>
+      <c r="M8" t="s">
         <v>320</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>321</v>
-      </c>
-      <c r="N8" t="s">
-        <v>322</v>
       </c>
       <c r="O8">
         <v>200300</v>
       </c>
       <c r="P8" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="Q8">
         <v>2121212121</v>
@@ -4702,7 +4777,7 @@
         <v>4141414141</v>
       </c>
       <c r="T8" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="U8">
         <v>5151515151</v>
@@ -4712,49 +4787,49 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="B9" t="s">
+        <v>344</v>
+      </c>
+      <c r="C9" t="s">
         <v>345</v>
       </c>
-      <c r="C9" t="s">
-        <v>346</v>
-      </c>
       <c r="D9" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F9" t="s">
+        <v>323</v>
+      </c>
+      <c r="G9" t="s">
         <v>324</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>325</v>
       </c>
-      <c r="H9" t="s">
-        <v>326</v>
-      </c>
       <c r="I9" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="J9">
         <v>201301</v>
       </c>
       <c r="K9" t="s">
+        <v>326</v>
+      </c>
+      <c r="L9" t="s">
+        <v>369</v>
+      </c>
+      <c r="M9" t="s">
         <v>327</v>
       </c>
-      <c r="L9" t="s">
-        <v>370</v>
-      </c>
-      <c r="M9" t="s">
-        <v>328</v>
-      </c>
       <c r="N9" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="O9">
         <v>10016</v>
       </c>
       <c r="P9" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="Q9">
         <v>98765429</v>
@@ -4766,7 +4841,7 @@
         <v>4141414141</v>
       </c>
       <c r="T9" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="U9">
         <v>5151515151</v>
@@ -4776,49 +4851,49 @@
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="B10" t="s">
+        <v>344</v>
+      </c>
+      <c r="C10" t="s">
         <v>345</v>
       </c>
-      <c r="C10" t="s">
-        <v>346</v>
-      </c>
       <c r="D10" t="s">
-        <v>314</v>
+        <v>313</v>
       </c>
       <c r="F10" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="G10" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="I10" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="J10">
         <v>500700</v>
       </c>
       <c r="K10" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L10" t="s">
+        <v>330</v>
+      </c>
+      <c r="M10" t="s">
         <v>331</v>
       </c>
-      <c r="M10" t="s">
-        <v>332</v>
-      </c>
       <c r="N10" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="O10">
         <v>2834</v>
       </c>
       <c r="P10" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="Q10">
         <v>1629539588</v>
@@ -4830,7 +4905,7 @@
         <v>4141414141</v>
       </c>
       <c r="T10" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="U10">
         <v>5151515151</v>
@@ -4840,52 +4915,52 @@
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="B11" t="s">
+        <v>347</v>
+      </c>
+      <c r="C11" t="s">
         <v>348</v>
       </c>
-      <c r="C11" t="s">
-        <v>349</v>
-      </c>
       <c r="D11" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E11" t="s">
-        <v>447</v>
+        <v>446</v>
       </c>
       <c r="F11" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="G11" t="s">
+        <v>338</v>
+      </c>
+      <c r="H11" t="s">
+        <v>386</v>
+      </c>
+      <c r="I11" t="s">
         <v>339</v>
-      </c>
-      <c r="H11" t="s">
-        <v>387</v>
-      </c>
-      <c r="I11" t="s">
-        <v>340</v>
       </c>
       <c r="J11">
         <v>560003</v>
       </c>
       <c r="K11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="L11" t="s">
+        <v>338</v>
+      </c>
+      <c r="M11" t="s">
+        <v>386</v>
+      </c>
+      <c r="N11" t="s">
         <v>339</v>
-      </c>
-      <c r="M11" t="s">
-        <v>387</v>
-      </c>
-      <c r="N11" t="s">
-        <v>340</v>
       </c>
       <c r="O11">
         <v>560003</v>
       </c>
       <c r="P11" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="Q11">
         <v>9999999999</v>
@@ -4897,13 +4972,13 @@
         <v>9955875125</v>
       </c>
       <c r="T11" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="U11">
         <v>9595956632</v>
       </c>
       <c r="V11" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="AJ11" s="6"/>
       <c r="AK11"/>
@@ -4958,97 +5033,97 @@
         <v>20</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C2" t="s">
         <v>72</v>
       </c>
-      <c r="C2" t="s">
-        <v>73</v>
-      </c>
       <c r="D2" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="E2">
         <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>469</v>
+        <v>506</v>
       </c>
       <c r="G2">
         <v>2019</v>
       </c>
       <c r="H2" t="s">
-        <v>452</v>
+        <v>492</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E3">
         <v>100</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G3">
         <v>2020</v>
       </c>
       <c r="H3" t="s">
-        <v>452</v>
+        <v>492</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E4">
         <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>474</v>
+        <v>510</v>
       </c>
       <c r="G4">
         <v>2021</v>
       </c>
       <c r="H4" t="s">
-        <v>452</v>
+        <v>492</v>
       </c>
     </row>
   </sheetData>
@@ -5082,148 +5157,148 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="E1" s="8" t="s">
         <v>212</v>
       </c>
-      <c r="E1" s="8" t="s">
+      <c r="F1" s="5" t="s">
         <v>213</v>
       </c>
-      <c r="F1" s="5" t="s">
-        <v>214</v>
-      </c>
       <c r="G1" s="5" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B2" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D2" t="s">
         <v>34</v>
       </c>
       <c r="E2" t="s">
+        <v>215</v>
+      </c>
+      <c r="F2" t="s">
         <v>216</v>
-      </c>
-      <c r="F2" t="s">
-        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B3" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C3" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D3" t="s">
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F3" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>227</v>
+      </c>
+      <c r="B4" t="s">
         <v>228</v>
       </c>
-      <c r="B4" t="s">
-        <v>229</v>
-      </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F4" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="G4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D5" t="s">
         <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="F5" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D6" t="s">
         <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="G6" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C7" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D7" t="s">
         <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="G7" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
   </sheetData>
@@ -5250,31 +5325,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B2" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B3" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -5315,148 +5390,148 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
+        <v>168</v>
+      </c>
+      <c r="C1" s="11" t="s">
         <v>169</v>
       </c>
-      <c r="C1" s="11" t="s">
+      <c r="D1" s="11" t="s">
+        <v>175</v>
+      </c>
+      <c r="E1" s="11" t="s">
         <v>170</v>
       </c>
-      <c r="D1" s="11" t="s">
-        <v>176</v>
-      </c>
-      <c r="E1" s="11" t="s">
+      <c r="F1" s="11" t="s">
         <v>171</v>
       </c>
-      <c r="F1" s="11" t="s">
+      <c r="G1" s="11" t="s">
+        <v>148</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="I1" s="11" t="s">
         <v>172</v>
       </c>
-      <c r="G1" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>150</v>
-      </c>
-      <c r="I1" s="11" t="s">
+      <c r="J1" s="11" t="s">
         <v>173</v>
       </c>
-      <c r="J1" s="11" t="s">
+      <c r="K1" s="11" t="s">
         <v>174</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>175</v>
       </c>
       <c r="L1" s="11" t="s">
         <v>30</v>
       </c>
       <c r="M1" s="11" t="s">
+        <v>165</v>
+      </c>
+      <c r="N1" s="11" t="s">
         <v>166</v>
       </c>
-      <c r="N1" s="11" t="s">
-        <v>167</v>
-      </c>
       <c r="O1" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="P1" s="11" t="s">
         <v>177</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>150</v>
+      </c>
+      <c r="B2" t="s">
+        <v>452</v>
+      </c>
+      <c r="C2" t="s">
         <v>151</v>
       </c>
-      <c r="B2" t="s">
-        <v>453</v>
-      </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>152</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>153</v>
-      </c>
-      <c r="E2" t="s">
-        <v>154</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
+        <v>153</v>
+      </c>
+      <c r="H2" t="s">
         <v>154</v>
-      </c>
-      <c r="H2" t="s">
-        <v>155</v>
       </c>
       <c r="I2" t="s">
         <v>34</v>
       </c>
       <c r="J2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O2" t="s">
+        <v>178</v>
+      </c>
+      <c r="P2" t="s">
         <v>179</v>
-      </c>
-      <c r="P2" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>156</v>
+      </c>
+      <c r="B3" t="s">
+        <v>443</v>
+      </c>
+      <c r="C3" t="s">
         <v>157</v>
-      </c>
-      <c r="B3" t="s">
-        <v>444</v>
-      </c>
-      <c r="C3" t="s">
-        <v>158</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="H3" t="s">
+        <v>158</v>
+      </c>
+      <c r="I3" t="s">
         <v>159</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>160</v>
       </c>
-      <c r="J3" t="s">
+      <c r="K3" t="s">
         <v>161</v>
-      </c>
-      <c r="K3" t="s">
-        <v>162</v>
       </c>
       <c r="L3">
         <v>25</v>
       </c>
       <c r="M3" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="N3" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B4" t="s">
+        <v>444</v>
+      </c>
+      <c r="C4" t="s">
         <v>163</v>
       </c>
-      <c r="B4" t="s">
-        <v>445</v>
-      </c>
-      <c r="C4" t="s">
-        <v>164</v>
-      </c>
       <c r="G4" t="s">
+        <v>153</v>
+      </c>
+      <c r="H4" t="s">
         <v>154</v>
-      </c>
-      <c r="H4" t="s">
-        <v>155</v>
       </c>
       <c r="I4" t="s">
         <v>36</v>
       </c>
       <c r="J4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -5493,25 +5568,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>180</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="C1" s="3" t="s">
-        <v>133</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>132</v>
-      </c>
-      <c r="E1" s="3" t="s">
+      <c r="F1" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="F1" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="G1" s="3" t="s">
+      <c r="H1" s="3" t="s">
         <v>183</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>184</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>26</v>
@@ -5520,36 +5595,36 @@
         <v>33</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>184</v>
+      </c>
+      <c r="B2" t="s">
         <v>185</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>186</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>187</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>188</v>
       </c>
-      <c r="E2" t="s">
-        <v>189</v>
-      </c>
       <c r="F2" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G2">
         <v>201300</v>
       </c>
       <c r="H2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I2">
         <v>243634535</v>
@@ -5558,36 +5633,36 @@
         <v>8867765</v>
       </c>
       <c r="K2" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="L2" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>190</v>
+      </c>
+      <c r="B3" t="s">
         <v>191</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>192</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>193</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F3" t="s">
         <v>194</v>
-      </c>
-      <c r="E3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F3" t="s">
-        <v>195</v>
       </c>
       <c r="G3">
         <v>400523</v>
       </c>
       <c r="H3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I3">
         <v>599546546</v>
@@ -5596,36 +5671,36 @@
         <v>1084566</v>
       </c>
       <c r="K3" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="L3" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>196</v>
+      </c>
+      <c r="B4" t="s">
         <v>197</v>
       </c>
-      <c r="B4" t="s">
+      <c r="C4" t="s">
         <v>198</v>
       </c>
-      <c r="C4" t="s">
-        <v>199</v>
-      </c>
       <c r="D4" t="s">
+        <v>187</v>
+      </c>
+      <c r="E4" t="s">
         <v>188</v>
       </c>
-      <c r="E4" t="s">
-        <v>189</v>
-      </c>
       <c r="F4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G4">
         <v>500900</v>
       </c>
       <c r="H4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="I4">
         <v>745465656</v>
@@ -5634,7 +5709,7 @@
         <v>45654656</v>
       </c>
       <c r="K4" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Revert "Acutiy 1.0 related changes"
This reverts commit 6661515275314e49ddf18fff2466276eb44e08a8.
</commit_message>
<xml_diff>
--- a/SmokeTestCases.xlsx
+++ b/SmokeTestCases.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView tabRatio="622" windowHeight="11160" windowWidth="20730" xWindow="-120" yWindow="-120"/>
+    <workbookView activeTab="18" firstSheet="13" tabRatio="622" windowHeight="11160" windowWidth="20730" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="Institutions" r:id="rId1" sheetId="22"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="864" uniqueCount="487">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -184,6 +184,9 @@
     <t>TestM1Institution2</t>
   </si>
   <si>
+    <t>Individual Investor</t>
+  </si>
+  <si>
     <t>TestM1Company1</t>
   </si>
   <si>
@@ -1432,12 +1435,27 @@
     <t>TestCompany1 - Feb 2022</t>
   </si>
   <si>
+    <t>PETestEmailFolder90700</t>
+  </si>
+  <si>
+    <t>PETestCustomEmailTemplate25516</t>
+  </si>
+  <si>
+    <t>navatariptesting+84488@gmail.com</t>
+  </si>
+  <si>
     <t>navatariptesting+14032@gmail.com</t>
   </si>
   <si>
     <t>navatariptesting+49277@gmail.com</t>
   </si>
   <si>
+    <t>navatariptesting+54430@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+40025@gmail.com</t>
+  </si>
+  <si>
     <t>7/20/2022</t>
   </si>
   <si>
@@ -1510,103 +1528,10 @@
     <t>ID-0632</t>
   </si>
   <si>
-    <t>CustomReportFolder34737</t>
-  </si>
-  <si>
-    <t>CustomReport44208</t>
-  </si>
-  <si>
-    <t>PETestEmailFolder47379</t>
-  </si>
-  <si>
-    <t>PETestCustomEmailTemplate59619</t>
-  </si>
-  <si>
-    <t>navatariptesting+93803@gmail.com</t>
-  </si>
-  <si>
-    <t>navatariptesting+66562@gmail.com</t>
-  </si>
-  <si>
-    <t>navatariptesting+8075@gmail.com</t>
-  </si>
-  <si>
-    <t>navatariptesting+11803@gmail.com</t>
-  </si>
-  <si>
-    <t>navatariptesting+19040@gmail.com</t>
-  </si>
-  <si>
-    <t>navatariptesting+20511@gmail.com</t>
-  </si>
-  <si>
-    <t>navatariptesting+29440@gmail.com</t>
-  </si>
-  <si>
-    <t>navatariptesting+37761@gmail.com</t>
-  </si>
-  <si>
-    <t>navatariptesting+10459@gmail.com</t>
-  </si>
-  <si>
-    <t>9/20/2022</t>
-  </si>
-  <si>
-    <t>navatariptesting+38840@gmail.com</t>
-  </si>
-  <si>
-    <t>navatariptesting+91042@gmail.com</t>
-  </si>
-  <si>
-    <t>navatariptesting+94321@gmail.com</t>
-  </si>
-  <si>
-    <t>navatariptesting+52197@gmail.com</t>
-  </si>
-  <si>
-    <t>navatariptesting+4134@gmail.com</t>
-  </si>
-  <si>
-    <t>6.3E8</t>
-  </si>
-  <si>
-    <t>9/21/2022</t>
-  </si>
-  <si>
-    <t>9/22/2022</t>
-  </si>
-  <si>
-    <t>CMT - 000950</t>
-  </si>
-  <si>
-    <t>CMT - 000951</t>
-  </si>
-  <si>
-    <t>6.7E8</t>
-  </si>
-  <si>
-    <t>9/24/2022</t>
-  </si>
-  <si>
-    <t>9/25/2022</t>
-  </si>
-  <si>
-    <t>6.75E8</t>
-  </si>
-  <si>
-    <t>9/28/2022</t>
-  </si>
-  <si>
-    <t>7.2E7</t>
-  </si>
-  <si>
-    <t>10/1/2022</t>
-  </si>
-  <si>
-    <t>8.4E7</t>
-  </si>
-  <si>
-    <t>10/6/2022</t>
+    <t>CustomReportFolder47527</t>
+  </si>
+  <si>
+    <t>CustomReport57424</t>
   </si>
 </sst>
 </file>
@@ -2033,9 +1958,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane activePane="bottomLeft" state="frozen" topLeftCell="A2" ySplit="1"/>
-      <selection activeCell="B13" pane="bottomLeft" sqref="B13"/>
+      <selection activeCell="A9" pane="bottomLeft" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2075,10 +2000,10 @@
         <v>29</v>
       </c>
       <c r="D1" s="7" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>30</v>
@@ -2090,43 +2015,43 @@
         <v>32</v>
       </c>
       <c r="I1" s="7" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="J1" s="7" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="K1" s="7" t="s">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="L1" s="7" t="s">
+        <v>133</v>
+      </c>
+      <c r="M1" s="7" t="s">
         <v>132</v>
       </c>
-      <c r="M1" s="7" t="s">
-        <v>131</v>
-      </c>
       <c r="N1" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="O1" s="7" t="s">
+        <v>134</v>
+      </c>
+      <c r="P1" s="7" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q1" s="7" t="s">
+        <v>136</v>
+      </c>
+      <c r="R1" s="7" t="s">
+        <v>137</v>
+      </c>
+      <c r="S1" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="T1" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="O1" s="7" t="s">
-        <v>133</v>
-      </c>
-      <c r="P1" s="7" t="s">
-        <v>134</v>
-      </c>
-      <c r="Q1" s="7" t="s">
-        <v>135</v>
-      </c>
-      <c r="R1" s="7" t="s">
-        <v>136</v>
-      </c>
-      <c r="S1" s="7" t="s">
-        <v>56</v>
-      </c>
-      <c r="T1" s="7" t="s">
-        <v>57</v>
-      </c>
       <c r="U1" s="7" t="s">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="V1" s="7" t="s">
         <v>26</v>
@@ -2137,7 +2062,7 @@
     </row>
     <row r="2" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
@@ -2148,28 +2073,28 @@
     </row>
     <row r="3" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="B3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>
       </c>
       <c r="L3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="M3" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O3">
         <v>210310</v>
       </c>
       <c r="P3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="V3">
         <v>3636366336</v>
@@ -2180,10 +2105,10 @@
     </row>
     <row r="4" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="B4" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -2191,28 +2116,28 @@
     </row>
     <row r="5" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="B5" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C5" t="s">
         <v>35</v>
       </c>
       <c r="L5" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="M5" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="N5" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O5">
         <v>900268</v>
       </c>
       <c r="P5" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="V5">
         <v>66228811</v>
@@ -2223,10 +2148,10 @@
     </row>
     <row r="6" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="C6" t="s">
         <v>35</v>
@@ -2234,169 +2159,169 @@
     </row>
     <row r="7" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="B7" t="s">
         <v>36</v>
       </c>
       <c r="C7" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="9" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="B9" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="C9" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B11" t="s">
+        <v>40</v>
+      </c>
+      <c r="C11" t="s">
         <v>39</v>
-      </c>
-      <c r="C11" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="B12" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C12" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H12" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="I12" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="J12" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="K12" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="L12" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="M12" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="N12" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="O12">
         <v>281001</v>
       </c>
       <c r="P12" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q12" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="R12" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="S12" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="T12">
         <v>200300</v>
       </c>
       <c r="U12" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="V12">
         <v>2121212121</v>
       </c>
       <c r="W12" s="15" t="s">
-        <v>368</v>
+        <v>369</v>
       </c>
     </row>
     <row r="13" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>341</v>
+        <v>342</v>
       </c>
       <c r="B13" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C13" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H13" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="I13" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="J13" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="K13" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="L13" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="M13" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="N13" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O13">
         <v>201301</v>
       </c>
       <c r="P13" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="Q13" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="R13" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="S13" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="T13">
         <v>10016</v>
       </c>
       <c r="U13" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="V13">
         <v>98765429</v>
@@ -2404,55 +2329,55 @@
     </row>
     <row r="14" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B14" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C14" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="H14" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="I14" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="J14" t="s">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="K14" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="L14" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="M14" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="N14" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="O14">
         <v>500700</v>
       </c>
       <c r="P14" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="Q14" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="R14" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="S14" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="T14">
         <v>2834</v>
       </c>
       <c r="U14" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="V14">
         <v>1629539588</v>
@@ -2460,58 +2385,58 @@
     </row>
     <row r="15" spans="1:23" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="B15" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="C15" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="H15" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="I15" t="s">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="J15" t="s">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="K15" t="s">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="L15" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="M15" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="N15" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="O15">
         <v>560003</v>
       </c>
       <c r="P15" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="Q15" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="R15" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="S15" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="T15">
         <v>560003</v>
       </c>
       <c r="U15" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="V15">
         <v>9999999999</v>
@@ -2554,54 +2479,54 @@
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>258</v>
+        <v>259</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="B2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="B3" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="C3" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D3" t="s">
-        <v>288</v>
+        <v>289</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B4" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="B5" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="C5" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -2650,135 +2575,135 @@
         <v>21</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="G1" s="3" t="s">
         <v>312</v>
       </c>
-      <c r="G1" s="3" t="s">
-        <v>311</v>
-      </c>
       <c r="H1" s="3" t="s">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="I1" s="3" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="K1" s="19" t="s">
-        <v>271</v>
+        <v>272</v>
       </c>
       <c r="L1" s="19" t="s">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="M1" s="19" t="s">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="N1" s="19" t="s">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="P1" s="3" t="s">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="Q1" s="16" t="s">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="R1" s="26" t="s">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="S1" s="16" t="s">
-        <v>410</v>
+        <v>411</v>
       </c>
       <c r="T1" s="3" t="s">
-        <v>277</v>
+        <v>278</v>
       </c>
     </row>
     <row r="2" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="B2" t="s">
-        <v>501</v>
+        <v>463</v>
       </c>
       <c r="C2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D2" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E2">
         <v>20000000</v>
       </c>
       <c r="F2" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="G2" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H2" t="s">
-        <v>499</v>
+        <v>461</v>
       </c>
       <c r="P2" s="18"/>
       <c r="T2" s="28" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>281</v>
+        <v>282</v>
       </c>
       <c r="B3" t="s">
-        <v>502</v>
+        <v>464</v>
       </c>
       <c r="C3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="D3" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E3">
         <v>10000000</v>
       </c>
       <c r="F3" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="G3" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H3" t="s">
-        <v>500</v>
+        <v>462</v>
       </c>
       <c r="T3" s="28"/>
     </row>
     <row r="4" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="B4" t="s">
-        <v>457</v>
+        <v>467</v>
       </c>
       <c r="C4" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D4" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E4">
         <v>15000000</v>
       </c>
       <c r="H4" t="s">
-        <v>504</v>
+        <v>465</v>
       </c>
       <c r="J4">
         <v>7.5</v>
@@ -2787,22 +2712,22 @@
     </row>
     <row r="5" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B5" t="s">
-        <v>458</v>
+        <v>468</v>
       </c>
       <c r="C5" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D5" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E5">
         <v>25000000</v>
       </c>
       <c r="H5" t="s">
-        <v>505</v>
+        <v>466</v>
       </c>
       <c r="J5">
         <v>7.5</v>
@@ -2811,100 +2736,100 @@
     </row>
     <row r="6" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B6" t="s">
-        <v>461</v>
+        <v>471</v>
       </c>
       <c r="C6" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D6" t="s">
-        <v>262</v>
+        <v>263</v>
       </c>
       <c r="E6">
         <v>5000000</v>
       </c>
       <c r="H6" t="s">
-        <v>507</v>
+        <v>470</v>
       </c>
       <c r="T6" s="28"/>
     </row>
     <row r="7" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="B7" t="s">
-        <v>462</v>
+        <v>473</v>
       </c>
       <c r="C7" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="D7" t="s">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="E7">
         <v>2000000</v>
       </c>
       <c r="H7" t="s">
-        <v>509</v>
+        <v>472</v>
       </c>
       <c r="I7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="T7" s="28"/>
     </row>
     <row r="8" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="B8" t="s">
-        <v>465</v>
+        <v>476</v>
       </c>
       <c r="C8" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="D8" t="s">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="E8">
         <v>12000000</v>
       </c>
       <c r="H8" t="s">
-        <v>511</v>
+        <v>475</v>
       </c>
       <c r="I8" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="T8" s="28"/>
     </row>
     <row r="9" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="B9" t="s">
-        <v>501</v>
+        <v>463</v>
       </c>
       <c r="C9" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D9" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E9">
         <v>20000000</v>
       </c>
       <c r="F9" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="G9" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H9" t="s">
-        <v>499</v>
+        <v>461</v>
       </c>
       <c r="K9" s="14" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="L9" s="14">
         <v>2000000</v>
@@ -2916,48 +2841,48 @@
         <v>0</v>
       </c>
       <c r="O9" s="14" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="P9" s="14">
         <v>0</v>
       </c>
       <c r="Q9" s="15" t="s">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="R9" s="15" t="s">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="S9">
         <v>0</v>
       </c>
       <c r="T9" t="s">
-        <v>283</v>
+        <v>284</v>
       </c>
     </row>
     <row r="10" spans="1:20" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="B10" t="s">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C10" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="D10" t="s">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="E10">
         <v>20000000</v>
       </c>
       <c r="F10" t="s">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="G10" t="s">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="H10" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="K10" s="15">
         <v>2000000</v>
@@ -2972,7 +2897,7 @@
         <v>0</v>
       </c>
       <c r="O10" s="14" t="s">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="P10" s="14">
         <v>0</v>
@@ -2987,7 +2912,7 @@
         <v>0</v>
       </c>
       <c r="T10" t="s">
-        <v>285</v>
+        <v>286</v>
       </c>
     </row>
   </sheetData>
@@ -3026,245 +2951,245 @@
         <v>0</v>
       </c>
       <c r="B1" s="19" t="s">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="D1" s="19" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="19" t="s">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="F1" s="19" t="s">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="G1" s="19" t="s">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="H1" s="19" t="s">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="I1" s="19" t="s">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="J1" s="19" t="s">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="K1" s="19" t="s">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="L1" s="19" t="s">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="M1" s="19" t="s">
-        <v>301</v>
+        <v>302</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="15" t="s">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="B2" t="s">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="C2" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="D2" t="s">
+        <v>468</v>
+      </c>
+      <c r="E2" t="s">
+        <v>375</v>
+      </c>
+      <c r="F2" t="s">
+        <v>382</v>
+      </c>
+      <c r="G2" t="s">
+        <v>382</v>
+      </c>
+      <c r="H2" t="s">
+        <v>383</v>
+      </c>
+      <c r="I2" t="s">
         <v>461</v>
       </c>
-      <c r="E2" t="s">
-        <v>422</v>
-      </c>
-      <c r="F2" t="s">
-        <v>423</v>
-      </c>
-      <c r="G2" t="s">
-        <v>423</v>
-      </c>
-      <c r="H2" t="s">
-        <v>424</v>
-      </c>
-      <c r="I2" t="s">
-        <v>499</v>
-      </c>
       <c r="J2" t="s">
-        <v>500</v>
+        <v>462</v>
       </c>
       <c r="K2" s="15" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="L2" s="21" t="s">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="M2" t="s">
-        <v>425</v>
+        <v>362</v>
       </c>
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="B3" t="s">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="C3" t="s">
+        <v>477</v>
+      </c>
+      <c r="D3" t="s">
         <v>471</v>
       </c>
-      <c r="D3" t="s">
-        <v>458</v>
-      </c>
       <c r="E3" t="s">
-        <v>374</v>
+        <v>423</v>
       </c>
       <c r="F3" t="s">
-        <v>381</v>
+        <v>424</v>
       </c>
       <c r="G3" t="s">
-        <v>381</v>
+        <v>424</v>
       </c>
       <c r="H3" t="s">
-        <v>382</v>
+        <v>425</v>
       </c>
       <c r="I3" t="s">
-        <v>499</v>
+        <v>461</v>
       </c>
       <c r="J3" t="s">
-        <v>500</v>
+        <v>462</v>
       </c>
       <c r="K3" s="15" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L3" s="15" t="s">
-        <v>359</v>
+        <v>360</v>
       </c>
       <c r="M3" t="s">
-        <v>361</v>
+        <v>426</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="B4" t="s">
-        <v>472</v>
+        <v>478</v>
       </c>
       <c r="C4" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="D4" t="s">
-        <v>501</v>
+        <v>463</v>
       </c>
       <c r="E4" t="s">
-        <v>372</v>
+        <v>373</v>
       </c>
       <c r="F4" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="G4" t="s">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="H4" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="I4" t="s">
-        <v>499</v>
+        <v>461</v>
       </c>
       <c r="J4" t="s">
-        <v>500</v>
+        <v>462</v>
       </c>
       <c r="K4" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="L4" t="s">
-        <v>499</v>
+        <v>461</v>
       </c>
       <c r="M4" t="s">
-        <v>356</v>
+        <v>357</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="B5" t="s">
-        <v>473</v>
+        <v>479</v>
       </c>
       <c r="C5" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="D5" t="s">
-        <v>502</v>
+        <v>464</v>
       </c>
       <c r="E5" t="s">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="F5" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="G5" t="s">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="H5" t="s">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="I5" t="s">
-        <v>499</v>
+        <v>461</v>
       </c>
       <c r="J5" t="s">
-        <v>500</v>
+        <v>462</v>
       </c>
       <c r="K5" s="14" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L5" s="14" t="s">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="M5" t="s">
-        <v>358</v>
+        <v>359</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
       <c r="B6" t="s">
-        <v>474</v>
+        <v>480</v>
       </c>
       <c r="C6" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="D6" t="s">
-        <v>457</v>
+        <v>467</v>
       </c>
       <c r="E6" t="s">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="F6" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="G6" t="s">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="H6" t="s">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="I6" t="s">
-        <v>499</v>
+        <v>461</v>
       </c>
       <c r="J6" t="s">
-        <v>500</v>
+        <v>462</v>
       </c>
       <c r="K6" s="15" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="L6" s="15" t="s">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="M6" t="s">
-        <v>360</v>
+        <v>361</v>
       </c>
     </row>
   </sheetData>
@@ -3299,66 +3224,66 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>384</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="K1" s="3" t="s">
         <v>296</v>
       </c>
-      <c r="E1" s="3" t="s">
-        <v>297</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>301</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>383</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>295</v>
-      </c>
       <c r="L1" s="3" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="M1" s="3" t="s">
-        <v>388</v>
+        <v>389</v>
       </c>
       <c r="N1" s="3" t="s">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="O1" s="3" t="s">
-        <v>393</v>
+        <v>394</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="B2" t="s">
-        <v>471</v>
+        <v>477</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D2" s="14" t="s">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="E2" t="s">
-        <v>499</v>
+        <v>461</v>
       </c>
       <c r="F2" t="s">
-        <v>500</v>
+        <v>462</v>
       </c>
       <c r="G2" s="14">
         <v>5500000</v>
@@ -3367,16 +3292,16 @@
         <v>2000000</v>
       </c>
       <c r="I2" s="14" t="s">
+        <v>392</v>
+      </c>
+      <c r="J2" s="14" t="s">
         <v>391</v>
-      </c>
-      <c r="J2" s="14" t="s">
-        <v>390</v>
       </c>
       <c r="K2" s="14">
         <v>750000</v>
       </c>
       <c r="L2" s="15" t="s">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="M2" s="15">
         <v>0</v>
@@ -3417,48 +3342,48 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="M1" s="3" t="s">
         <v>394</v>
-      </c>
-      <c r="E1" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="F1" s="3" t="s">
-        <v>298</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>294</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="K1" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="L1" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="B2" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="D2">
         <v>15000000</v>
@@ -3503,200 +3428,200 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>21</v>
       </c>
       <c r="E1" s="25" t="s">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="F1" s="3" t="s">
+        <v>395</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>396</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>397</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>398</v>
+      </c>
+      <c r="J1" s="3" t="s">
+        <v>399</v>
+      </c>
+      <c r="M1" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="O1" s="3" t="s">
         <v>394</v>
-      </c>
-      <c r="G1" s="3" t="s">
-        <v>395</v>
-      </c>
-      <c r="H1" s="3" t="s">
-        <v>396</v>
-      </c>
-      <c r="I1" s="3" t="s">
-        <v>397</v>
-      </c>
-      <c r="J1" s="3" t="s">
-        <v>398</v>
-      </c>
-      <c r="M1" s="3" t="s">
-        <v>388</v>
-      </c>
-      <c r="N1" s="3" t="s">
-        <v>389</v>
-      </c>
-      <c r="O1" s="3" t="s">
-        <v>393</v>
       </c>
     </row>
     <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="B2" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="C2" t="s">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="D2" t="s">
-        <v>461</v>
+        <v>468</v>
       </c>
       <c r="E2" t="s">
         <v>429</v>
       </c>
       <c r="F2" t="s">
-        <v>377</v>
+        <v>430</v>
       </c>
       <c r="G2" t="s">
+        <v>431</v>
+      </c>
+      <c r="H2" t="s">
+        <v>431</v>
+      </c>
+      <c r="I2" t="s">
+        <v>431</v>
+      </c>
+      <c r="J2" t="s">
         <v>432</v>
-      </c>
-      <c r="H2" t="s">
-        <v>432</v>
-      </c>
-      <c r="I2" t="s">
-        <v>432</v>
-      </c>
-      <c r="J2" t="s">
-        <v>433</v>
       </c>
     </row>
     <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>402</v>
+        <v>403</v>
       </c>
       <c r="B3" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="C3" t="s">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="D3" t="s">
-        <v>458</v>
+        <v>471</v>
       </c>
       <c r="E3" t="s">
-        <v>428</v>
+        <v>430</v>
       </c>
       <c r="F3" t="s">
-        <v>429</v>
+        <v>378</v>
       </c>
       <c r="G3" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="H3" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="I3" t="s">
-        <v>430</v>
+        <v>433</v>
       </c>
       <c r="J3" t="s">
-        <v>431</v>
+        <v>434</v>
       </c>
     </row>
     <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B4" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="C4" t="s">
-        <v>476</v>
+        <v>482</v>
       </c>
       <c r="D4" t="s">
-        <v>501</v>
+        <v>463</v>
       </c>
       <c r="E4" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="F4" t="s">
+        <v>409</v>
+      </c>
+      <c r="G4" t="s">
+        <v>435</v>
+      </c>
+      <c r="H4" t="s">
+        <v>435</v>
+      </c>
+      <c r="I4" t="s">
+        <v>435</v>
+      </c>
+      <c r="J4" t="s">
         <v>408</v>
-      </c>
-      <c r="G4" t="s">
-        <v>434</v>
-      </c>
-      <c r="H4" t="s">
-        <v>434</v>
-      </c>
-      <c r="I4" t="s">
-        <v>434</v>
-      </c>
-      <c r="J4" t="s">
-        <v>407</v>
       </c>
     </row>
     <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="B5" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="C5" t="s">
-        <v>477</v>
+        <v>483</v>
       </c>
       <c r="D5" t="s">
-        <v>502</v>
+        <v>464</v>
       </c>
       <c r="E5" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="F5" t="s">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="G5" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="H5" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="I5" t="s">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="J5" t="s">
-        <v>440</v>
+        <v>441</v>
       </c>
     </row>
     <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="B6" t="s">
-        <v>475</v>
+        <v>481</v>
       </c>
       <c r="C6" t="s">
-        <v>478</v>
+        <v>484</v>
       </c>
       <c r="D6" t="s">
-        <v>457</v>
+        <v>467</v>
       </c>
       <c r="E6" t="s">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="F6" t="s">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="G6" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="H6" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="I6" t="s">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="J6" t="s">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
   </sheetData>
@@ -3726,88 +3651,88 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>199</v>
+        <v>200</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>200</v>
+        <v>201</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>202</v>
+        <v>203</v>
       </c>
       <c r="B2" t="s">
-        <v>203</v>
+        <v>204</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>204</v>
+        <v>205</v>
       </c>
       <c r="B3" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="C3" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D3" t="s">
-        <v>206</v>
+        <v>207</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>207</v>
+        <v>208</v>
       </c>
       <c r="B4" t="s">
-        <v>208</v>
+        <v>209</v>
       </c>
       <c r="D4" t="s">
-        <v>209</v>
+        <v>210</v>
       </c>
       <c r="E4" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>231</v>
+        <v>232</v>
       </c>
       <c r="B5" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="B6" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
       <c r="C6" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="D6" t="s">
-        <v>235</v>
+        <v>236</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>236</v>
+        <v>237</v>
       </c>
       <c r="B7" t="s">
-        <v>237</v>
+        <v>238</v>
       </c>
       <c r="D7" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="E7" t="s">
-        <v>421</v>
+        <v>422</v>
       </c>
     </row>
   </sheetData>
@@ -3860,7 +3785,7 @@
         <v>25</v>
       </c>
       <c r="J1" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -3883,7 +3808,7 @@
         <v>10</v>
       </c>
       <c r="J2" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -3891,16 +3816,16 @@
         <v>12</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="C3" t="s">
         <v>11</v>
       </c>
       <c r="D3" t="s">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="E3" t="s">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="F3" t="s">
         <v>19</v>
@@ -3909,10 +3834,10 @@
         <v>10</v>
       </c>
       <c r="H3" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="I3" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -3955,57 +3880,57 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="G1" s="5" t="s">
         <v>32</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>126</v>
+        <v>127</v>
       </c>
       <c r="B2" t="s">
-        <v>481</v>
+        <v>454</v>
       </c>
       <c r="C2" t="s">
-        <v>482</v>
+        <v>455</v>
       </c>
       <c r="D2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="F2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="G2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="H2" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="I2" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
     </row>
     <row customHeight="1" ht="15" r="6" spans="1:9" x14ac:dyDescent="0.25"/>
@@ -4018,7 +3943,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
@@ -4038,19 +3963,19 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="G1" s="5"/>
       <c r="H1" s="5"/>
@@ -4058,22 +3983,22 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>479</v>
+        <v>485</v>
       </c>
       <c r="C2" t="s">
-        <v>480</v>
+        <v>486</v>
       </c>
       <c r="D2" t="s">
-        <v>449</v>
+        <v>450</v>
       </c>
       <c r="E2" t="s">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="F2" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>
@@ -4109,86 +4034,86 @@
         <v>1</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>31</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>308</v>
+        <v>309</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>245</v>
+        <v>246</v>
       </c>
       <c r="B2" t="s">
         <v>34</v>
       </c>
       <c r="C2" t="s">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="E2" s="20" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F2" t="s">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="X2" s="27" t="s">
-        <v>247</v>
+        <v>248</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="B3" t="s">
         <v>34</v>
       </c>
       <c r="C3" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="E3" s="20" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F3" t="s">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="X3" s="27"/>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="B4" t="s">
         <v>34</v>
       </c>
       <c r="C4" t="s">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="D4" t="s">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="E4" s="20" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="X4" s="27"/>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="B5" t="s">
         <v>36</v>
       </c>
       <c r="C5" t="s">
-        <v>254</v>
+        <v>255</v>
       </c>
       <c r="E5" s="20" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="F5">
         <v>5000000</v>
@@ -4197,16 +4122,16 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B6" t="s">
         <v>36</v>
       </c>
       <c r="C6" t="s">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="E6" s="20" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="X6" s="27"/>
     </row>
@@ -4243,10 +4168,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>2</v>
@@ -4258,91 +4183,91 @@
         <v>7</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>219</v>
+        <v>220</v>
       </c>
       <c r="I1" s="5" t="s">
         <v>26</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>220</v>
+        <v>221</v>
       </c>
       <c r="B2" t="s">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D2" t="s">
         <v>11</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="F2" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="G2" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="H2" t="s">
         <v>34</v>
       </c>
       <c r="J2" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>221</v>
+        <v>222</v>
       </c>
       <c r="B3" t="s">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D3" t="s">
         <v>11</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G3" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H3" t="s">
         <v>36</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>223</v>
+        <v>224</v>
       </c>
       <c r="B4" t="s">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C4" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="D4" t="s">
         <v>11</v>
       </c>
       <c r="E4" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G4" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H4" t="s">
         <v>36</v>
@@ -4350,48 +4275,48 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>225</v>
+        <v>226</v>
       </c>
       <c r="B5" t="s">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D5" t="s">
         <v>11</v>
       </c>
       <c r="E5" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G5" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H5" t="s">
         <v>36</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="B6" t="s">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="D6" t="s">
         <v>11</v>
       </c>
       <c r="E6" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G6" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H6" t="s">
         <v>36</v>
@@ -4399,74 +4324,74 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>241</v>
+        <v>242</v>
       </c>
       <c r="B7" t="s">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="C7" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="D7" t="s">
         <v>11</v>
       </c>
       <c r="E7" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="G7" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H7" t="s">
         <v>34</v>
       </c>
       <c r="J7" t="s">
-        <v>453</v>
+        <v>457</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="B8" t="s">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="C8" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D8" t="s">
         <v>11</v>
       </c>
       <c r="E8" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="G8" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H8" t="s">
         <v>36</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>454</v>
+        <v>458</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="B9" t="s">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="C9" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="D9" t="s">
         <v>11</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="G9" t="s">
-        <v>222</v>
+        <v>223</v>
       </c>
       <c r="H9" t="s">
         <v>36</v>
@@ -4561,43 +4486,43 @@
         <v>28</v>
       </c>
       <c r="J1" s="5" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="K1" s="5" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="L1" s="5" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="M1" s="5" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="N1" s="8" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O1" s="8" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="P1" s="5" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="Q1" s="5" t="s">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="R1" s="5" t="s">
         <v>33</v>
       </c>
       <c r="S1" s="5" t="s">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="T1" s="5" t="s">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="U1" s="5" t="s">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="V1" s="5" t="s">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="W1" s="5" t="s">
         <v>29</v>
@@ -4606,64 +4531,64 @@
     </row>
     <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="B2" t="s">
         <v>11</v>
       </c>
       <c r="C2" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D2" t="s">
         <v>34</v>
       </c>
-      <c r="E2" t="s">
-        <v>495</v>
+      <c r="E2" s="2" t="s">
+        <v>457</v>
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="B3" t="s">
         <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="D3" t="s">
         <v>34</v>
       </c>
-      <c r="E3" t="s">
-        <v>496</v>
+      <c r="E3" s="2" t="s">
+        <v>456</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="B4" t="s">
         <v>11</v>
       </c>
       <c r="C4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="D4" t="s">
         <v>36</v>
       </c>
-      <c r="E4" t="s">
-        <v>497</v>
+      <c r="E4" s="2" t="s">
+        <v>458</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="B5" t="s">
         <v>11</v>
       </c>
       <c r="C5" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="D5" t="s">
         <v>36</v>
@@ -4671,101 +4596,101 @@
     </row>
     <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="B6" t="s">
         <v>11</v>
       </c>
       <c r="C6" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="D6" t="s">
-        <v>40</v>
-      </c>
-      <c r="E6" t="s">
-        <v>493</v>
+        <v>41</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>459</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="B7" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C7" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="D7" t="s">
-        <v>47</v>
-      </c>
-      <c r="E7" t="s">
-        <v>494</v>
+        <v>48</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>460</v>
       </c>
       <c r="L7" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="M7" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="N7" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="O7">
         <v>654927</v>
       </c>
       <c r="P7" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
     </row>
     <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="B8" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C8" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D8" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="E8" t="s">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="F8" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="G8" t="s">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="H8" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I8" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="J8">
         <v>281001</v>
       </c>
       <c r="K8" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L8" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="M8" t="s">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="N8" t="s">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="O8">
         <v>200300</v>
       </c>
       <c r="P8" t="s">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="Q8">
         <v>2121212121</v>
@@ -4777,7 +4702,7 @@
         <v>4141414141</v>
       </c>
       <c r="T8" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="U8">
         <v>5151515151</v>
@@ -4787,49 +4712,49 @@
     </row>
     <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="B9" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C9" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D9" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F9" t="s">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="G9" t="s">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="H9" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="I9" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="J9">
         <v>201301</v>
       </c>
       <c r="K9" t="s">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="L9" t="s">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="M9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="N9" t="s">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="O9">
         <v>10016</v>
       </c>
       <c r="P9" t="s">
-        <v>328</v>
+        <v>329</v>
       </c>
       <c r="Q9">
         <v>98765429</v>
@@ -4841,7 +4766,7 @@
         <v>4141414141</v>
       </c>
       <c r="T9" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="U9">
         <v>5151515151</v>
@@ -4851,49 +4776,49 @@
     </row>
     <row r="10" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>352</v>
+        <v>353</v>
       </c>
       <c r="B10" t="s">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="C10" t="s">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="D10" t="s">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="F10" t="s">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="G10" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="H10" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="I10" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="J10">
         <v>500700</v>
       </c>
       <c r="K10" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L10" t="s">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M10" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="N10" t="s">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="O10">
         <v>2834</v>
       </c>
       <c r="P10" t="s">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="Q10">
         <v>1629539588</v>
@@ -4905,7 +4830,7 @@
         <v>4141414141</v>
       </c>
       <c r="T10" t="s">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="U10">
         <v>5151515151</v>
@@ -4915,52 +4840,52 @@
     </row>
     <row r="11" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B11" t="s">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="C11" t="s">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="D11" t="s">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="E11" t="s">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="F11" t="s">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="G11" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="H11" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="I11" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="J11">
         <v>560003</v>
       </c>
       <c r="K11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="L11" t="s">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="M11" t="s">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="N11" t="s">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="O11">
         <v>560003</v>
       </c>
       <c r="P11" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="Q11">
         <v>9999999999</v>
@@ -4972,13 +4897,13 @@
         <v>9955875125</v>
       </c>
       <c r="T11" t="s">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="U11">
         <v>9595956632</v>
       </c>
       <c r="V11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="AJ11" s="6"/>
       <c r="AK11"/>
@@ -5033,97 +4958,97 @@
         <v>20</v>
       </c>
       <c r="D1" s="8" t="s">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="E1" s="5" t="s">
-        <v>127</v>
+        <v>128</v>
       </c>
       <c r="F1" s="22" t="s">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="H1" s="9" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>128</v>
+        <v>129</v>
       </c>
       <c r="B2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D2" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="E2">
         <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>506</v>
+        <v>469</v>
       </c>
       <c r="G2">
         <v>2019</v>
       </c>
       <c r="H2" t="s">
-        <v>492</v>
+        <v>452</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>129</v>
+        <v>130</v>
       </c>
       <c r="B3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" t="s">
         <v>73</v>
       </c>
-      <c r="C3" t="s">
-        <v>72</v>
-      </c>
       <c r="D3" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E3">
         <v>100</v>
       </c>
       <c r="F3" s="24" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G3">
         <v>2020</v>
       </c>
       <c r="H3" t="s">
-        <v>492</v>
+        <v>452</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>130</v>
+        <v>131</v>
       </c>
       <c r="B4" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="D4" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="E4">
         <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>510</v>
+        <v>474</v>
       </c>
       <c r="G4">
         <v>2021</v>
       </c>
       <c r="H4" t="s">
-        <v>492</v>
+        <v>452</v>
       </c>
     </row>
   </sheetData>
@@ -5157,148 +5082,148 @@
         <v>0</v>
       </c>
       <c r="B1" s="8" t="s">
-        <v>210</v>
+        <v>211</v>
       </c>
       <c r="C1" s="5" t="s">
         <v>5</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>211</v>
+        <v>212</v>
       </c>
       <c r="E1" s="8" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>213</v>
+        <v>214</v>
       </c>
       <c r="G1" s="5" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="B2" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="C2" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="D2" t="s">
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F2" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>217</v>
+        <v>218</v>
       </c>
       <c r="B3" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C3" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D3" t="s">
         <v>36</v>
       </c>
       <c r="E3" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F3" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>227</v>
+        <v>228</v>
       </c>
       <c r="B4" t="s">
-        <v>228</v>
+        <v>229</v>
       </c>
       <c r="C4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D4" t="s">
         <v>34</v>
       </c>
       <c r="E4" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F4" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="G4" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>230</v>
+        <v>231</v>
       </c>
       <c r="B5" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="D5" t="s">
         <v>36</v>
       </c>
       <c r="E5" t="s">
-        <v>215</v>
+        <v>216</v>
       </c>
       <c r="F5" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G5" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>239</v>
+        <v>240</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C6" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D6" t="s">
         <v>34</v>
       </c>
       <c r="F6" t="s">
-        <v>216</v>
+        <v>217</v>
       </c>
       <c r="G6" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
       <c r="B7" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C7" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="D7" t="s">
         <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>218</v>
+        <v>219</v>
       </c>
       <c r="G7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
   </sheetData>
@@ -5325,31 +5250,31 @@
         <v>0</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B2" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="B3" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -5390,148 +5315,148 @@
         <v>0</v>
       </c>
       <c r="B1" s="11" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C1" s="11" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="D1" s="11" t="s">
+        <v>176</v>
+      </c>
+      <c r="E1" s="11" t="s">
+        <v>171</v>
+      </c>
+      <c r="F1" s="11" t="s">
+        <v>172</v>
+      </c>
+      <c r="G1" s="11" t="s">
+        <v>149</v>
+      </c>
+      <c r="H1" s="11" t="s">
+        <v>150</v>
+      </c>
+      <c r="I1" s="11" t="s">
+        <v>173</v>
+      </c>
+      <c r="J1" s="11" t="s">
+        <v>174</v>
+      </c>
+      <c r="K1" s="11" t="s">
         <v>175</v>
-      </c>
-      <c r="E1" s="11" t="s">
-        <v>170</v>
-      </c>
-      <c r="F1" s="11" t="s">
-        <v>171</v>
-      </c>
-      <c r="G1" s="11" t="s">
-        <v>148</v>
-      </c>
-      <c r="H1" s="11" t="s">
-        <v>149</v>
-      </c>
-      <c r="I1" s="11" t="s">
-        <v>172</v>
-      </c>
-      <c r="J1" s="11" t="s">
-        <v>173</v>
-      </c>
-      <c r="K1" s="11" t="s">
-        <v>174</v>
       </c>
       <c r="L1" s="11" t="s">
         <v>30</v>
       </c>
       <c r="M1" s="11" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="N1" s="11" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="O1" s="11" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="P1" s="11" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="B2" t="s">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="C2" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="D2" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="E2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="F2">
         <v>0</v>
       </c>
       <c r="G2" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H2" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I2" t="s">
         <v>34</v>
       </c>
       <c r="J2" t="s">
-        <v>155</v>
+        <v>156</v>
       </c>
       <c r="O2" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="P2" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B3" t="s">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="C3" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="F3">
         <v>0</v>
       </c>
       <c r="G3" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H3" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="I3" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="J3" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="K3" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="L3">
         <v>25</v>
       </c>
       <c r="M3" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="N3" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B4" t="s">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="C4" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="G4" t="s">
-        <v>153</v>
+        <v>154</v>
       </c>
       <c r="H4" t="s">
-        <v>154</v>
+        <v>155</v>
       </c>
       <c r="I4" t="s">
         <v>36</v>
       </c>
       <c r="J4" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>
@@ -5568,25 +5493,25 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="C1" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="D1" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="D1" s="3" t="s">
-        <v>131</v>
-      </c>
       <c r="E1" s="3" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="F1" s="3" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="G1" s="3" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="H1" s="3" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="I1" s="3" t="s">
         <v>26</v>
@@ -5595,36 +5520,36 @@
         <v>33</v>
       </c>
       <c r="K1" s="3" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="L1" s="4" t="s">
-        <v>224</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B2" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C2" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="D2" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E2" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F2" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G2">
         <v>201300</v>
       </c>
       <c r="H2" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I2">
         <v>243634535</v>
@@ -5633,36 +5558,36 @@
         <v>8867765</v>
       </c>
       <c r="K2" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="L2" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B3" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C3" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="D3" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="E3" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="F3" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="G3">
         <v>400523</v>
       </c>
       <c r="H3" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I3">
         <v>599546546</v>
@@ -5671,36 +5596,36 @@
         <v>1084566</v>
       </c>
       <c r="K3" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="L3" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>197</v>
       </c>
       <c r="B4" t="s">
-        <v>197</v>
+        <v>198</v>
       </c>
       <c r="C4" t="s">
-        <v>198</v>
+        <v>199</v>
       </c>
       <c r="D4" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="E4" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="F4" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="G4">
         <v>500900</v>
       </c>
       <c r="H4" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="I4">
         <v>745465656</v>
@@ -5709,7 +5634,7 @@
         <v>45654656</v>
       </c>
       <c r="K4" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Acuity changes phase 1
Signed-off-by: Testing <rkumar1@navatargroup.com>
</commit_message>
<xml_diff>
--- a/SmokeTestCases.xlsx
+++ b/SmokeTestCases.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1014" uniqueCount="512">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1324" uniqueCount="572">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -1607,6 +1607,186 @@
   </si>
   <si>
     <t>10/6/2022</t>
+  </si>
+  <si>
+    <t>CustomReportFolder92078</t>
+  </si>
+  <si>
+    <t>CustomReport19181</t>
+  </si>
+  <si>
+    <t>PETestEmailFolder40186</t>
+  </si>
+  <si>
+    <t>PETestCustomEmailTemplate26009</t>
+  </si>
+  <si>
+    <t>navatariptesting+47248@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+5398@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+75684@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+32815@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+44643@gmail.com</t>
+  </si>
+  <si>
+    <t>10/13/2022</t>
+  </si>
+  <si>
+    <t>7.05E8</t>
+  </si>
+  <si>
+    <t>10/14/2022</t>
+  </si>
+  <si>
+    <t>7.45E8</t>
+  </si>
+  <si>
+    <t>10/16/2022</t>
+  </si>
+  <si>
+    <t>10/17/2022</t>
+  </si>
+  <si>
+    <t>7.5E8</t>
+  </si>
+  <si>
+    <t>10/21/2022</t>
+  </si>
+  <si>
+    <t>8.6E7</t>
+  </si>
+  <si>
+    <t>10/24/2022</t>
+  </si>
+  <si>
+    <t>9.8E7</t>
+  </si>
+  <si>
+    <t>10/29/2022</t>
+  </si>
+  <si>
+    <t>10/18/2022</t>
+  </si>
+  <si>
+    <t>CustomReportFolder7404</t>
+  </si>
+  <si>
+    <t>CustomReport53088</t>
+  </si>
+  <si>
+    <t>PETestEmailFolder23854</t>
+  </si>
+  <si>
+    <t>PETestCustomEmailTemplate37534</t>
+  </si>
+  <si>
+    <t>navatariptesting+25845@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+27632@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+59874@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+45689@gmail.com</t>
+  </si>
+  <si>
+    <t>navatariptesting+41597@gmail.com</t>
+  </si>
+  <si>
+    <t>7.8E8</t>
+  </si>
+  <si>
+    <t>10/22/2022</t>
+  </si>
+  <si>
+    <t>8.2E8</t>
+  </si>
+  <si>
+    <t>10/28/2022</t>
+  </si>
+  <si>
+    <t>CMT - 000959</t>
+  </si>
+  <si>
+    <t>CMT - 000960</t>
+  </si>
+  <si>
+    <t>8.25E8</t>
+  </si>
+  <si>
+    <t>11/1/2022</t>
+  </si>
+  <si>
+    <t>CMT - 000961</t>
+  </si>
+  <si>
+    <t>1.0E8</t>
+  </si>
+  <si>
+    <t>11/4/2022</t>
+  </si>
+  <si>
+    <t>CMT - 000962</t>
+  </si>
+  <si>
+    <t>1.12E8</t>
+  </si>
+  <si>
+    <t>11/9/2022</t>
+  </si>
+  <si>
+    <t>CMT - 000963</t>
+  </si>
+  <si>
+    <t>10/25/2022</t>
+  </si>
+  <si>
+    <t>10/26/2022</t>
+  </si>
+  <si>
+    <t>DD-0217</t>
+  </si>
+  <si>
+    <t>CC-0627</t>
+  </si>
+  <si>
+    <t>CC-0628</t>
+  </si>
+  <si>
+    <t>CC-0629</t>
+  </si>
+  <si>
+    <t>CC-0630</t>
+  </si>
+  <si>
+    <t>CC-0631</t>
+  </si>
+  <si>
+    <t>FD-0230</t>
+  </si>
+  <si>
+    <t>ID-0633</t>
+  </si>
+  <si>
+    <t>ID-0634</t>
+  </si>
+  <si>
+    <t>ID-0635</t>
+  </si>
+  <si>
+    <t>ID-0636</t>
+  </si>
+  <si>
+    <t>ID-0637</t>
   </si>
 </sst>
 </file>
@@ -2709,7 +2889,7 @@
         <v>278</v>
       </c>
       <c r="B2" t="s">
-        <v>501</v>
+        <v>467</v>
       </c>
       <c r="C2" t="s">
         <v>246</v>
@@ -2727,7 +2907,7 @@
         <v>280</v>
       </c>
       <c r="H2" t="s">
-        <v>499</v>
+        <v>528</v>
       </c>
       <c r="P2" s="18"/>
       <c r="T2" s="28" t="s">
@@ -2739,7 +2919,7 @@
         <v>281</v>
       </c>
       <c r="B3" t="s">
-        <v>502</v>
+        <v>470</v>
       </c>
       <c r="C3" t="s">
         <v>249</v>
@@ -2757,7 +2937,7 @@
         <v>280</v>
       </c>
       <c r="H3" t="s">
-        <v>500</v>
+        <v>544</v>
       </c>
       <c r="T3" s="28"/>
     </row>
@@ -2766,7 +2946,7 @@
         <v>286</v>
       </c>
       <c r="B4" t="s">
-        <v>457</v>
+        <v>547</v>
       </c>
       <c r="C4" t="s">
         <v>246</v>
@@ -2778,7 +2958,7 @@
         <v>15000000</v>
       </c>
       <c r="H4" t="s">
-        <v>504</v>
+        <v>546</v>
       </c>
       <c r="J4">
         <v>7.5</v>
@@ -2790,7 +2970,7 @@
         <v>287</v>
       </c>
       <c r="B5" t="s">
-        <v>458</v>
+        <v>548</v>
       </c>
       <c r="C5" t="s">
         <v>251</v>
@@ -2802,7 +2982,7 @@
         <v>25000000</v>
       </c>
       <c r="H5" t="s">
-        <v>505</v>
+        <v>532</v>
       </c>
       <c r="J5">
         <v>7.5</v>
@@ -2814,7 +2994,7 @@
         <v>289</v>
       </c>
       <c r="B6" t="s">
-        <v>461</v>
+        <v>551</v>
       </c>
       <c r="C6" t="s">
         <v>254</v>
@@ -2826,7 +3006,7 @@
         <v>5000000</v>
       </c>
       <c r="H6" t="s">
-        <v>507</v>
+        <v>550</v>
       </c>
       <c r="T6" s="28"/>
     </row>
@@ -2835,7 +3015,7 @@
         <v>309</v>
       </c>
       <c r="B7" t="s">
-        <v>462</v>
+        <v>554</v>
       </c>
       <c r="C7" t="s">
         <v>254</v>
@@ -2847,7 +3027,7 @@
         <v>2000000</v>
       </c>
       <c r="H7" t="s">
-        <v>509</v>
+        <v>553</v>
       </c>
       <c r="I7" t="s">
         <v>39</v>
@@ -2859,7 +3039,7 @@
         <v>387</v>
       </c>
       <c r="B8" t="s">
-        <v>465</v>
+        <v>557</v>
       </c>
       <c r="C8" t="s">
         <v>256</v>
@@ -2871,7 +3051,7 @@
         <v>12000000</v>
       </c>
       <c r="H8" t="s">
-        <v>511</v>
+        <v>556</v>
       </c>
       <c r="I8" t="s">
         <v>39</v>
@@ -2883,7 +3063,7 @@
         <v>370</v>
       </c>
       <c r="B9" t="s">
-        <v>501</v>
+        <v>467</v>
       </c>
       <c r="C9" t="s">
         <v>246</v>
@@ -2901,7 +3081,7 @@
         <v>280</v>
       </c>
       <c r="H9" t="s">
-        <v>499</v>
+        <v>528</v>
       </c>
       <c r="K9" s="14" t="s">
         <v>374</v>
@@ -3067,13 +3247,13 @@
         <v>302</v>
       </c>
       <c r="B2" t="s">
-        <v>426</v>
+        <v>561</v>
       </c>
       <c r="C2" t="s">
-        <v>471</v>
+        <v>560</v>
       </c>
       <c r="D2" t="s">
-        <v>461</v>
+        <v>551</v>
       </c>
       <c r="E2" t="s">
         <v>422</v>
@@ -3088,16 +3268,16 @@
         <v>424</v>
       </c>
       <c r="I2" t="s">
-        <v>499</v>
+        <v>558</v>
       </c>
       <c r="J2" t="s">
-        <v>500</v>
-      </c>
-      <c r="K2" s="15" t="s">
+        <v>559</v>
+      </c>
+      <c r="K2" t="s">
         <v>374</v>
       </c>
-      <c r="L2" s="21" t="s">
-        <v>357</v>
+      <c r="L2" t="s">
+        <v>526</v>
       </c>
       <c r="M2" t="s">
         <v>425</v>
@@ -3108,13 +3288,13 @@
         <v>303</v>
       </c>
       <c r="B3" t="s">
-        <v>427</v>
+        <v>562</v>
       </c>
       <c r="C3" t="s">
-        <v>471</v>
+        <v>560</v>
       </c>
       <c r="D3" t="s">
-        <v>458</v>
+        <v>548</v>
       </c>
       <c r="E3" t="s">
         <v>374</v>
@@ -3129,10 +3309,10 @@
         <v>382</v>
       </c>
       <c r="I3" t="s">
-        <v>499</v>
+        <v>558</v>
       </c>
       <c r="J3" t="s">
-        <v>500</v>
+        <v>559</v>
       </c>
       <c r="K3" s="15" t="s">
         <v>229</v>
@@ -3149,13 +3329,13 @@
         <v>304</v>
       </c>
       <c r="B4" t="s">
-        <v>472</v>
+        <v>563</v>
       </c>
       <c r="C4" t="s">
-        <v>471</v>
+        <v>560</v>
       </c>
       <c r="D4" t="s">
-        <v>501</v>
+        <v>467</v>
       </c>
       <c r="E4" t="s">
         <v>372</v>
@@ -3170,16 +3350,16 @@
         <v>374</v>
       </c>
       <c r="I4" t="s">
-        <v>499</v>
+        <v>558</v>
       </c>
       <c r="J4" t="s">
-        <v>500</v>
+        <v>559</v>
       </c>
       <c r="K4" t="s">
         <v>374</v>
       </c>
       <c r="L4" t="s">
-        <v>499</v>
+        <v>558</v>
       </c>
       <c r="M4" t="s">
         <v>356</v>
@@ -3190,13 +3370,13 @@
         <v>305</v>
       </c>
       <c r="B5" t="s">
-        <v>473</v>
+        <v>564</v>
       </c>
       <c r="C5" t="s">
-        <v>471</v>
+        <v>560</v>
       </c>
       <c r="D5" t="s">
-        <v>502</v>
+        <v>470</v>
       </c>
       <c r="E5" t="s">
         <v>375</v>
@@ -3211,10 +3391,10 @@
         <v>377</v>
       </c>
       <c r="I5" t="s">
-        <v>499</v>
+        <v>558</v>
       </c>
       <c r="J5" t="s">
-        <v>500</v>
+        <v>559</v>
       </c>
       <c r="K5" s="14" t="s">
         <v>229</v>
@@ -3231,13 +3411,13 @@
         <v>306</v>
       </c>
       <c r="B6" t="s">
-        <v>474</v>
+        <v>565</v>
       </c>
       <c r="C6" t="s">
-        <v>471</v>
+        <v>560</v>
       </c>
       <c r="D6" t="s">
-        <v>457</v>
+        <v>547</v>
       </c>
       <c r="E6" t="s">
         <v>378</v>
@@ -3252,10 +3432,10 @@
         <v>380</v>
       </c>
       <c r="I6" t="s">
-        <v>499</v>
+        <v>558</v>
       </c>
       <c r="J6" t="s">
-        <v>500</v>
+        <v>559</v>
       </c>
       <c r="K6" s="15" t="s">
         <v>229</v>
@@ -3346,7 +3526,7 @@
         <v>291</v>
       </c>
       <c r="B2" t="s">
-        <v>471</v>
+        <v>560</v>
       </c>
       <c r="C2" t="s">
         <v>71</v>
@@ -3355,10 +3535,10 @@
         <v>384</v>
       </c>
       <c r="E2" t="s">
-        <v>499</v>
+        <v>558</v>
       </c>
       <c r="F2" t="s">
-        <v>500</v>
+        <v>559</v>
       </c>
       <c r="G2" s="14">
         <v>5500000</v>
@@ -3458,7 +3638,7 @@
         <v>406</v>
       </c>
       <c r="B2" t="s">
-        <v>475</v>
+        <v>566</v>
       </c>
       <c r="D2">
         <v>15000000</v>
@@ -3544,13 +3724,13 @@
         <v>401</v>
       </c>
       <c r="B2" t="s">
-        <v>475</v>
+        <v>566</v>
       </c>
       <c r="C2" t="s">
-        <v>441</v>
+        <v>567</v>
       </c>
       <c r="D2" t="s">
-        <v>461</v>
+        <v>551</v>
       </c>
       <c r="E2" t="s">
         <v>429</v>
@@ -3576,13 +3756,13 @@
         <v>402</v>
       </c>
       <c r="B3" t="s">
-        <v>475</v>
+        <v>566</v>
       </c>
       <c r="C3" t="s">
-        <v>442</v>
+        <v>568</v>
       </c>
       <c r="D3" t="s">
-        <v>458</v>
+        <v>548</v>
       </c>
       <c r="E3" t="s">
         <v>428</v>
@@ -3608,13 +3788,13 @@
         <v>403</v>
       </c>
       <c r="B4" t="s">
-        <v>475</v>
+        <v>566</v>
       </c>
       <c r="C4" t="s">
-        <v>476</v>
+        <v>569</v>
       </c>
       <c r="D4" t="s">
-        <v>501</v>
+        <v>467</v>
       </c>
       <c r="E4" t="s">
         <v>419</v>
@@ -3640,13 +3820,13 @@
         <v>404</v>
       </c>
       <c r="B5" t="s">
-        <v>475</v>
+        <v>566</v>
       </c>
       <c r="C5" t="s">
-        <v>477</v>
+        <v>570</v>
       </c>
       <c r="D5" t="s">
-        <v>502</v>
+        <v>470</v>
       </c>
       <c r="E5" t="s">
         <v>420</v>
@@ -3672,13 +3852,13 @@
         <v>405</v>
       </c>
       <c r="B6" t="s">
-        <v>475</v>
+        <v>566</v>
       </c>
       <c r="C6" t="s">
-        <v>478</v>
+        <v>571</v>
       </c>
       <c r="D6" t="s">
-        <v>457</v>
+        <v>547</v>
       </c>
       <c r="E6" t="s">
         <v>435</v>
@@ -3984,10 +4164,10 @@
         <v>126</v>
       </c>
       <c r="B2" t="s">
-        <v>481</v>
+        <v>536</v>
       </c>
       <c r="C2" t="s">
-        <v>482</v>
+        <v>537</v>
       </c>
       <c r="D2" t="s">
         <v>109</v>
@@ -4061,10 +4241,10 @@
         <v>125</v>
       </c>
       <c r="B2" t="s">
-        <v>479</v>
+        <v>534</v>
       </c>
       <c r="C2" t="s">
-        <v>480</v>
+        <v>535</v>
       </c>
       <c r="D2" t="s">
         <v>449</v>
@@ -4618,7 +4798,7 @@
         <v>34</v>
       </c>
       <c r="E2" t="s">
-        <v>495</v>
+        <v>540</v>
       </c>
     </row>
     <row r="3" spans="1:38" x14ac:dyDescent="0.25">
@@ -4635,7 +4815,7 @@
         <v>34</v>
       </c>
       <c r="E3" t="s">
-        <v>496</v>
+        <v>541</v>
       </c>
     </row>
     <row r="4" spans="1:38" x14ac:dyDescent="0.25">
@@ -4652,7 +4832,7 @@
         <v>36</v>
       </c>
       <c r="E4" t="s">
-        <v>497</v>
+        <v>542</v>
       </c>
     </row>
     <row r="5" spans="1:38" x14ac:dyDescent="0.25">
@@ -4683,7 +4863,7 @@
         <v>40</v>
       </c>
       <c r="E6" t="s">
-        <v>493</v>
+        <v>538</v>
       </c>
     </row>
     <row r="7" spans="1:38" x14ac:dyDescent="0.25">
@@ -4700,7 +4880,7 @@
         <v>47</v>
       </c>
       <c r="E7" t="s">
-        <v>494</v>
+        <v>539</v>
       </c>
       <c r="L7" t="s">
         <v>66</v>
@@ -5065,13 +5245,13 @@
         <v>100</v>
       </c>
       <c r="F2" t="s">
-        <v>506</v>
+        <v>549</v>
       </c>
       <c r="G2">
         <v>2019</v>
       </c>
       <c r="H2" t="s">
-        <v>492</v>
+        <v>528</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
@@ -5097,7 +5277,7 @@
         <v>2020</v>
       </c>
       <c r="H3" t="s">
-        <v>492</v>
+        <v>528</v>
       </c>
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.25">
@@ -5117,13 +5297,13 @@
         <v>100</v>
       </c>
       <c r="F4" t="s">
-        <v>510</v>
+        <v>555</v>
       </c>
       <c r="G4">
         <v>2021</v>
       </c>
       <c r="H4" t="s">
-        <v>492</v>
+        <v>528</v>
       </c>
     </row>
   </sheetData>

</xml_diff>